<commit_message>
Adding model fits to plots for pasture meter and grass chem responses
</commit_message>
<xml_diff>
--- a/outputs/SupplementalTables.xlsx
+++ b/outputs/SupplementalTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\AppraisingGrazing\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D6B748-D447-45F4-801B-F4D5A027B13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E9E7B5-6069-4405-BEFA-8BFAF5DA6282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="4" xr2:uid="{CF962987-2438-4E1C-BBD3-768B42620E9E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="5" xr2:uid="{CF962987-2438-4E1C-BBD3-768B42620E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="SiteDescriptions" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ElementGradient" sheetId="2" r:id="rId3"/>
     <sheet name="BiomassTRT" sheetId="3" r:id="rId4"/>
     <sheet name="BiomassGradient" sheetId="4" r:id="rId5"/>
+    <sheet name="BiomassPerTRT" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="93">
   <si>
     <t>bison</t>
   </si>
@@ -480,7 +481,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,15 +644,21 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -661,17 +668,65 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1491,7 +1546,7 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+      <selection activeCell="M3" sqref="M3:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,10 +1568,10 @@
       <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="58" t="s">
         <v>92</v>
       </c>
       <c r="D1" s="24" t="s">
@@ -1537,10 +1592,10 @@
       <c r="J1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="58" t="s">
         <v>92</v>
       </c>
       <c r="M1" s="24" t="s">
@@ -1561,10 +1616,10 @@
       <c r="S1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="60" t="s">
+      <c r="T1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="58" t="s">
         <v>92</v>
       </c>
       <c r="V1" s="24" t="s">
@@ -1584,11 +1639,11 @@
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1604,11 +1659,11 @@
       <c r="H2" s="15">
         <v>0.75643309065928399</v>
       </c>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
       <c r="M2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1624,11 +1679,11 @@
       <c r="Q2" s="15">
         <v>0.78445569199090504</v>
       </c>
-      <c r="S2" s="61" t="s">
+      <c r="S2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1646,7 +1701,7 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
       <c r="D3" s="13" t="s">
@@ -1664,7 +1719,7 @@
       <c r="H3" s="15">
         <v>0.85620580622572096</v>
       </c>
-      <c r="J3" s="62"/>
+      <c r="J3" s="64"/>
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
       <c r="M3" s="13" t="s">
@@ -1682,7 +1737,7 @@
       <c r="Q3" s="15">
         <v>0.111358770556964</v>
       </c>
-      <c r="S3" s="62"/>
+      <c r="S3" s="64"/>
       <c r="T3" s="44"/>
       <c r="U3" s="44"/>
       <c r="V3" s="13" t="s">
@@ -1702,7 +1757,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="44">
         <v>0.59</v>
       </c>
@@ -1724,7 +1779,7 @@
       <c r="H4" s="15">
         <v>0.198730750798048</v>
       </c>
-      <c r="J4" s="62"/>
+      <c r="J4" s="64"/>
       <c r="K4" s="44">
         <v>0.41</v>
       </c>
@@ -1746,7 +1801,7 @@
       <c r="Q4" s="15">
         <v>0.54152757122083806</v>
       </c>
-      <c r="S4" s="62"/>
+      <c r="S4" s="64"/>
       <c r="T4" s="44">
         <v>0.21</v>
       </c>
@@ -1770,7 +1825,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="13" t="s">
@@ -1788,7 +1843,7 @@
       <c r="H5" s="22">
         <v>2.0426214511249902E-2</v>
       </c>
-      <c r="J5" s="62"/>
+      <c r="J5" s="64"/>
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
       <c r="M5" s="13" t="s">
@@ -1806,7 +1861,7 @@
       <c r="Q5" s="15">
         <v>0.58620851191461298</v>
       </c>
-      <c r="S5" s="62"/>
+      <c r="S5" s="64"/>
       <c r="T5" s="44"/>
       <c r="U5" s="44"/>
       <c r="V5" s="13" t="s">
@@ -1826,7 +1881,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="63"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
       <c r="D6" s="16" t="s">
@@ -1844,7 +1899,7 @@
       <c r="H6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="63"/>
+      <c r="J6" s="65"/>
       <c r="K6" s="45"/>
       <c r="L6" s="45"/>
       <c r="M6" s="16" t="s">
@@ -1862,7 +1917,7 @@
       <c r="Q6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="63"/>
+      <c r="S6" s="65"/>
       <c r="T6" s="45"/>
       <c r="U6" s="45"/>
       <c r="V6" s="16" t="s">
@@ -1882,11 +1937,11 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1902,11 +1957,11 @@
       <c r="H7" s="5">
         <v>0.45450659664544801</v>
       </c>
-      <c r="J7" s="64" t="s">
+      <c r="J7" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
       <c r="M7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1922,11 +1977,11 @@
       <c r="Q7" s="5">
         <v>0.96017688602466</v>
       </c>
-      <c r="S7" s="64" t="s">
+      <c r="S7" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="T7" s="59"/>
-      <c r="U7" s="59"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
       <c r="V7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1944,7 +1999,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="3" t="s">
@@ -1962,7 +2017,7 @@
       <c r="H8" s="5">
         <v>0.53062471950727597</v>
       </c>
-      <c r="J8" s="65"/>
+      <c r="J8" s="61"/>
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="3" t="s">
@@ -1980,7 +2035,7 @@
       <c r="Q8" s="5">
         <v>0.49430589283329901</v>
       </c>
-      <c r="S8" s="65"/>
+      <c r="S8" s="61"/>
       <c r="T8" s="41"/>
       <c r="U8" s="41"/>
       <c r="V8" s="3" t="s">
@@ -2000,7 +2055,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="41">
         <v>0.23</v>
       </c>
@@ -2022,7 +2077,7 @@
       <c r="H9" s="5">
         <v>0.85845654845826103</v>
       </c>
-      <c r="J9" s="65"/>
+      <c r="J9" s="61"/>
       <c r="K9" s="41">
         <v>0.32</v>
       </c>
@@ -2044,7 +2099,7 @@
       <c r="Q9" s="5">
         <v>0.12333957548581399</v>
       </c>
-      <c r="S9" s="65"/>
+      <c r="S9" s="61"/>
       <c r="T9" s="41">
         <v>0.21</v>
       </c>
@@ -2068,7 +2123,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="3" t="s">
@@ -2086,7 +2141,7 @@
       <c r="H10" s="5">
         <v>0.68725480675239803</v>
       </c>
-      <c r="J10" s="65"/>
+      <c r="J10" s="61"/>
       <c r="K10" s="41"/>
       <c r="L10" s="41"/>
       <c r="M10" s="3" t="s">
@@ -2104,7 +2159,7 @@
       <c r="Q10" s="5">
         <v>0.56468785934212196</v>
       </c>
-      <c r="S10" s="65"/>
+      <c r="S10" s="61"/>
       <c r="T10" s="41"/>
       <c r="U10" s="41"/>
       <c r="V10" s="3" t="s">
@@ -2124,7 +2179,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="66"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
       <c r="D11" s="6" t="s">
@@ -2142,7 +2197,7 @@
       <c r="H11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="66"/>
+      <c r="J11" s="62"/>
       <c r="K11" s="42"/>
       <c r="L11" s="42"/>
       <c r="M11" s="6" t="s">
@@ -2160,7 +2215,7 @@
       <c r="Q11" s="12">
         <v>5.6703110896494401E-4</v>
       </c>
-      <c r="S11" s="66"/>
+      <c r="S11" s="62"/>
       <c r="T11" s="42"/>
       <c r="U11" s="42"/>
       <c r="V11" s="6" t="s">
@@ -2181,11 +2236,11 @@
       <c r="AF11" s="35"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="13" t="s">
         <v>0</v>
       </c>
@@ -2201,11 +2256,11 @@
       <c r="H12" s="15">
         <v>0.70634877764113901</v>
       </c>
-      <c r="J12" s="61" t="s">
+      <c r="J12" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
       <c r="M12" s="13" t="s">
         <v>0</v>
       </c>
@@ -2221,11 +2276,11 @@
       <c r="Q12" s="15">
         <v>0.96903819673954605</v>
       </c>
-      <c r="S12" s="61" t="s">
+      <c r="S12" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="44"/>
       <c r="V12" s="13" t="s">
         <v>0</v>
       </c>
@@ -2243,7 +2298,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
@@ -2261,7 +2316,7 @@
       <c r="H13" s="15">
         <v>0.98064258715030805</v>
       </c>
-      <c r="J13" s="62"/>
+      <c r="J13" s="64"/>
       <c r="K13" s="44"/>
       <c r="L13" s="44"/>
       <c r="M13" s="13" t="s">
@@ -2279,7 +2334,7 @@
       <c r="Q13" s="15">
         <v>0.204959108693586</v>
       </c>
-      <c r="S13" s="62"/>
+      <c r="S13" s="64"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
       <c r="V13" s="13" t="s">
@@ -2299,7 +2354,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="44">
         <v>0.36</v>
       </c>
@@ -2321,7 +2376,7 @@
       <c r="H14" s="15">
         <v>0.46443467686441597</v>
       </c>
-      <c r="J14" s="62"/>
+      <c r="J14" s="64"/>
       <c r="K14" s="44">
         <v>0.33</v>
       </c>
@@ -2343,7 +2398,7 @@
       <c r="Q14" s="15">
         <v>0.28711644693738703</v>
       </c>
-      <c r="S14" s="62"/>
+      <c r="S14" s="64"/>
       <c r="T14" s="44">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2367,7 +2422,7 @@
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
       <c r="D15" s="13" t="s">
@@ -2385,7 +2440,7 @@
       <c r="H15" s="15">
         <v>0.17886255886840399</v>
       </c>
-      <c r="J15" s="62"/>
+      <c r="J15" s="64"/>
       <c r="K15" s="44"/>
       <c r="L15" s="44"/>
       <c r="M15" s="13" t="s">
@@ -2403,7 +2458,7 @@
       <c r="Q15" s="15">
         <v>0.43957422325523998</v>
       </c>
-      <c r="S15" s="62"/>
+      <c r="S15" s="64"/>
       <c r="T15" s="44"/>
       <c r="U15" s="44"/>
       <c r="V15" s="13" t="s">
@@ -2423,7 +2478,7 @@
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" s="63"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
       <c r="D16" s="16" t="s">
@@ -2441,7 +2496,7 @@
       <c r="H16" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="63"/>
+      <c r="J16" s="65"/>
       <c r="K16" s="45"/>
       <c r="L16" s="45"/>
       <c r="M16" s="16" t="s">
@@ -2459,7 +2514,7 @@
       <c r="Q16" s="19">
         <v>9.5878767935397803E-4</v>
       </c>
-      <c r="S16" s="63"/>
+      <c r="S16" s="65"/>
       <c r="T16" s="45"/>
       <c r="U16" s="45"/>
       <c r="V16" s="16" t="s">
@@ -2480,11 +2535,11 @@
       <c r="AF16" s="35"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="3" t="s">
         <v>0</v>
       </c>
@@ -2500,11 +2555,11 @@
       <c r="H17" s="10">
         <v>4.2440815812778497E-2</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="J17" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
       <c r="M17" s="3" t="s">
         <v>0</v>
       </c>
@@ -2520,11 +2575,11 @@
       <c r="Q17" s="5">
         <v>0.50381674695789302</v>
       </c>
-      <c r="S17" s="64" t="s">
+      <c r="S17" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="T17" s="59"/>
-      <c r="U17" s="59"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
       <c r="V17" s="3" t="s">
         <v>0</v>
       </c>
@@ -2542,7 +2597,7 @@
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="3" t="s">
@@ -2560,7 +2615,7 @@
       <c r="H18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="65"/>
+      <c r="J18" s="61"/>
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="3" t="s">
@@ -2578,7 +2633,7 @@
       <c r="Q18" s="5">
         <v>0.264487950777611</v>
       </c>
-      <c r="S18" s="65"/>
+      <c r="S18" s="61"/>
       <c r="T18" s="41"/>
       <c r="U18" s="41"/>
       <c r="V18" s="3" t="s">
@@ -2598,7 +2653,7 @@
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="41">
         <v>0.31</v>
       </c>
@@ -2620,7 +2675,7 @@
       <c r="H19" s="5">
         <v>9.6818088993625706E-2</v>
       </c>
-      <c r="J19" s="65"/>
+      <c r="J19" s="61"/>
       <c r="K19" s="41">
         <v>0.26</v>
       </c>
@@ -2642,7 +2697,7 @@
       <c r="Q19" s="5">
         <v>0.37610715062244399</v>
       </c>
-      <c r="S19" s="65"/>
+      <c r="S19" s="61"/>
       <c r="T19" s="41">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2666,7 +2721,7 @@
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="3" t="s">
@@ -2684,7 +2739,7 @@
       <c r="H20" s="10">
         <v>6.5707623725130805E-4</v>
       </c>
-      <c r="J20" s="65"/>
+      <c r="J20" s="61"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="3" t="s">
@@ -2702,7 +2757,7 @@
       <c r="Q20" s="5">
         <v>0.239285481771352</v>
       </c>
-      <c r="S20" s="65"/>
+      <c r="S20" s="61"/>
       <c r="T20" s="41"/>
       <c r="U20" s="41"/>
       <c r="V20" s="3" t="s">
@@ -2722,7 +2777,7 @@
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A21" s="66"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="6" t="s">
@@ -2740,7 +2795,7 @@
       <c r="H21" s="12">
         <v>5.7643528578590598E-2</v>
       </c>
-      <c r="J21" s="66"/>
+      <c r="J21" s="62"/>
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
       <c r="M21" s="6" t="s">
@@ -2758,7 +2813,7 @@
       <c r="Q21" s="8">
         <v>0.18897297602503599</v>
       </c>
-      <c r="S21" s="66"/>
+      <c r="S21" s="62"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
       <c r="V21" s="6" t="s">
@@ -2778,11 +2833,11 @@
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="13" t="s">
         <v>0</v>
       </c>
@@ -2798,11 +2853,11 @@
       <c r="H22" s="15">
         <v>5.8951439115694199E-2</v>
       </c>
-      <c r="J22" s="61" t="s">
+      <c r="J22" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
       <c r="M22" s="13" t="s">
         <v>0</v>
       </c>
@@ -2818,11 +2873,11 @@
       <c r="Q22" s="15">
         <v>0.85580186913876699</v>
       </c>
-      <c r="S22" s="61" t="s">
+      <c r="S22" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="44"/>
       <c r="V22" s="13" t="s">
         <v>0</v>
       </c>
@@ -2840,7 +2895,7 @@
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
       <c r="D23" s="13" t="s">
@@ -2858,7 +2913,7 @@
       <c r="H23" s="15">
         <v>0.898896282859034</v>
       </c>
-      <c r="J23" s="62"/>
+      <c r="J23" s="64"/>
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
       <c r="M23" s="13" t="s">
@@ -2876,7 +2931,7 @@
       <c r="Q23" s="15">
         <v>0.53963880509304496</v>
       </c>
-      <c r="S23" s="62"/>
+      <c r="S23" s="64"/>
       <c r="T23" s="44"/>
       <c r="U23" s="44"/>
       <c r="V23" s="13" t="s">
@@ -2896,7 +2951,7 @@
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="44">
         <v>0.13</v>
       </c>
@@ -2918,7 +2973,7 @@
       <c r="H24" s="15">
         <v>0.56247855473640496</v>
       </c>
-      <c r="J24" s="62"/>
+      <c r="J24" s="64"/>
       <c r="K24" s="44">
         <v>0.27</v>
       </c>
@@ -2940,7 +2995,7 @@
       <c r="Q24" s="15">
         <v>0.19620110579128799</v>
       </c>
-      <c r="S24" s="62"/>
+      <c r="S24" s="64"/>
       <c r="T24" s="44">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2964,7 +3019,7 @@
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A25" s="62"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="13" t="s">
@@ -2982,7 +3037,7 @@
       <c r="H25" s="15">
         <v>0.96061530261722605</v>
       </c>
-      <c r="J25" s="62"/>
+      <c r="J25" s="64"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="13" t="s">
@@ -3000,7 +3055,7 @@
       <c r="Q25" s="15">
         <v>0.57714986420537495</v>
       </c>
-      <c r="S25" s="62"/>
+      <c r="S25" s="64"/>
       <c r="T25" s="44"/>
       <c r="U25" s="44"/>
       <c r="V25" s="13" t="s">
@@ -3020,7 +3075,7 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
       <c r="D26" s="16" t="s">
@@ -3038,7 +3093,7 @@
       <c r="H26" s="20">
         <v>0.32774660012482898</v>
       </c>
-      <c r="J26" s="63"/>
+      <c r="J26" s="65"/>
       <c r="K26" s="45"/>
       <c r="L26" s="45"/>
       <c r="M26" s="16" t="s">
@@ -3056,7 +3111,7 @@
       <c r="Q26" s="20">
         <v>0.21330625309083201</v>
       </c>
-      <c r="S26" s="63"/>
+      <c r="S26" s="65"/>
       <c r="T26" s="45"/>
       <c r="U26" s="45"/>
       <c r="V26" s="16" t="s">
@@ -3076,11 +3131,11 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
       <c r="D27" s="3" t="s">
         <v>0</v>
       </c>
@@ -3096,11 +3151,11 @@
       <c r="H27" s="10">
         <v>4.0137352839097598E-2</v>
       </c>
-      <c r="J27" s="64" t="s">
+      <c r="J27" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
       <c r="M27" s="3" t="s">
         <v>0</v>
       </c>
@@ -3116,11 +3171,11 @@
       <c r="Q27" s="5">
         <v>0.65952820034885495</v>
       </c>
-      <c r="S27" s="64" t="s">
+      <c r="S27" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
       <c r="V27" s="3" t="s">
         <v>0</v>
       </c>
@@ -3138,7 +3193,7 @@
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
       <c r="D28" s="3" t="s">
@@ -3156,7 +3211,7 @@
       <c r="H28" s="10">
         <v>3.5068868917491801E-2</v>
       </c>
-      <c r="J28" s="65"/>
+      <c r="J28" s="61"/>
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="3" t="s">
@@ -3174,7 +3229,7 @@
       <c r="Q28" s="5">
         <v>0.94359388051558002</v>
       </c>
-      <c r="S28" s="65"/>
+      <c r="S28" s="61"/>
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="V28" s="3" t="s">
@@ -3194,7 +3249,7 @@
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="41">
         <v>0.71</v>
       </c>
@@ -3216,7 +3271,7 @@
       <c r="H29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="65"/>
+      <c r="J29" s="61"/>
       <c r="K29" s="41">
         <v>0.68</v>
       </c>
@@ -3238,7 +3293,7 @@
       <c r="Q29" s="5">
         <v>0.96316540129969996</v>
       </c>
-      <c r="S29" s="65"/>
+      <c r="S29" s="61"/>
       <c r="T29" s="41">
         <v>0.05</v>
       </c>
@@ -3263,7 +3318,7 @@
       <c r="AF29" s="35"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
       <c r="D30" s="3" t="s">
@@ -3281,7 +3336,7 @@
       <c r="H30" s="5">
         <v>7.7615500578327001E-2</v>
       </c>
-      <c r="J30" s="65"/>
+      <c r="J30" s="61"/>
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="3" t="s">
@@ -3299,7 +3354,7 @@
       <c r="Q30" s="5">
         <v>0.83562337156051503</v>
       </c>
-      <c r="S30" s="65"/>
+      <c r="S30" s="61"/>
       <c r="T30" s="41"/>
       <c r="U30" s="41"/>
       <c r="V30" s="3" t="s">
@@ -3319,7 +3374,7 @@
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A31" s="66"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
       <c r="D31" s="6" t="s">
@@ -3337,7 +3392,7 @@
       <c r="H31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="66"/>
+      <c r="J31" s="62"/>
       <c r="K31" s="42"/>
       <c r="L31" s="42"/>
       <c r="M31" s="6" t="s">
@@ -3355,7 +3410,7 @@
       <c r="Q31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="S31" s="66"/>
+      <c r="S31" s="62"/>
       <c r="T31" s="42"/>
       <c r="U31" s="42"/>
       <c r="V31" s="6" t="s">
@@ -3380,12 +3435,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
     <mergeCell ref="S27:S31"/>
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="J7:J11"/>
@@ -3398,6 +3447,12 @@
     <mergeCell ref="S12:S16"/>
     <mergeCell ref="S17:S21"/>
     <mergeCell ref="S22:S26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3409,7 +3464,7 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3428,10 +3483,10 @@
       <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="58" t="s">
         <v>92</v>
       </c>
       <c r="D1" s="24" t="s">
@@ -3452,10 +3507,10 @@
       <c r="J1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="58" t="s">
         <v>92</v>
       </c>
       <c r="M1" s="24" t="s">
@@ -3476,10 +3531,10 @@
       <c r="S1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="60" t="s">
+      <c r="T1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="58" t="s">
         <v>92</v>
       </c>
       <c r="V1" s="24" t="s">
@@ -3499,11 +3554,11 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="34" t="s">
         <v>0</v>
       </c>
@@ -3519,7 +3574,7 @@
       <c r="H2" s="26">
         <v>0.232594480943555</v>
       </c>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="63" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="43"/>
@@ -3539,7 +3594,7 @@
       <c r="Q2" s="26">
         <v>0.58051575449478299</v>
       </c>
-      <c r="S2" s="61" t="s">
+      <c r="S2" s="63" t="s">
         <v>20</v>
       </c>
       <c r="T2" s="43"/>
@@ -3561,7 +3616,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
       <c r="D3" s="13" t="s">
@@ -3579,7 +3634,7 @@
       <c r="H3" s="15">
         <v>0.72085458380743095</v>
       </c>
-      <c r="J3" s="62"/>
+      <c r="J3" s="64"/>
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
       <c r="M3" s="13" t="s">
@@ -3597,7 +3652,7 @@
       <c r="Q3" s="15">
         <v>0.22034570029552</v>
       </c>
-      <c r="S3" s="62"/>
+      <c r="S3" s="64"/>
       <c r="T3" s="44"/>
       <c r="U3" s="44"/>
       <c r="V3" s="13" t="s">
@@ -3617,7 +3672,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="44">
         <v>0.7</v>
       </c>
@@ -3639,7 +3694,7 @@
       <c r="H4" s="22">
         <v>1.62257649215358E-3</v>
       </c>
-      <c r="J4" s="62"/>
+      <c r="J4" s="64"/>
       <c r="K4" s="44">
         <v>0.41</v>
       </c>
@@ -3661,7 +3716,7 @@
       <c r="Q4" s="15">
         <v>0.45992161771271001</v>
       </c>
-      <c r="S4" s="62"/>
+      <c r="S4" s="64"/>
       <c r="T4" s="44">
         <v>0.44</v>
       </c>
@@ -3685,7 +3740,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="13" t="s">
@@ -3703,7 +3758,7 @@
       <c r="H5" s="15">
         <v>0.90736653483351304</v>
       </c>
-      <c r="J5" s="62"/>
+      <c r="J5" s="64"/>
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
       <c r="M5" s="13" t="s">
@@ -3721,7 +3776,7 @@
       <c r="Q5" s="15">
         <v>0.49155219186801202</v>
       </c>
-      <c r="S5" s="62"/>
+      <c r="S5" s="64"/>
       <c r="T5" s="44"/>
       <c r="U5" s="44"/>
       <c r="V5" s="13" t="s">
@@ -3741,7 +3796,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="63"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
       <c r="D6" s="16" t="s">
@@ -3759,7 +3814,7 @@
       <c r="H6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="63"/>
+      <c r="J6" s="65"/>
       <c r="K6" s="45"/>
       <c r="L6" s="45"/>
       <c r="M6" s="16" t="s">
@@ -3777,7 +3832,7 @@
       <c r="Q6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="63"/>
+      <c r="S6" s="65"/>
       <c r="T6" s="45"/>
       <c r="U6" s="45"/>
       <c r="V6" s="16" t="s">
@@ -3797,11 +3852,11 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="36" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3872,7 @@
       <c r="H7" s="27">
         <v>0.552259009406043</v>
       </c>
-      <c r="J7" s="64" t="s">
+      <c r="J7" s="60" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="40"/>
@@ -3837,7 +3892,7 @@
       <c r="Q7" s="27">
         <v>0.32181313500870801</v>
       </c>
-      <c r="S7" s="64" t="s">
+      <c r="S7" s="60" t="s">
         <v>21</v>
       </c>
       <c r="T7" s="40"/>
@@ -3859,7 +3914,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="3" t="s">
@@ -3877,7 +3932,7 @@
       <c r="H8" s="5">
         <v>0.32335190904313799</v>
       </c>
-      <c r="J8" s="65"/>
+      <c r="J8" s="61"/>
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="3" t="s">
@@ -3895,7 +3950,7 @@
       <c r="Q8" s="5">
         <v>0.85330548504150305</v>
       </c>
-      <c r="S8" s="65"/>
+      <c r="S8" s="61"/>
       <c r="T8" s="41"/>
       <c r="U8" s="41"/>
       <c r="V8" s="3" t="s">
@@ -3915,7 +3970,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="41">
         <v>0.39</v>
       </c>
@@ -3937,7 +3992,7 @@
       <c r="H9" s="5">
         <v>0.124419258908589</v>
       </c>
-      <c r="J9" s="65"/>
+      <c r="J9" s="61"/>
       <c r="K9" s="41">
         <v>0.2</v>
       </c>
@@ -3959,7 +4014,7 @@
       <c r="Q9" s="5">
         <v>0.46405023322165001</v>
       </c>
-      <c r="S9" s="65"/>
+      <c r="S9" s="61"/>
       <c r="T9" s="41">
         <v>0.46</v>
       </c>
@@ -3983,7 +4038,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="3" t="s">
@@ -4001,7 +4056,7 @@
       <c r="H10" s="5">
         <v>0.65137158175371701</v>
       </c>
-      <c r="J10" s="65"/>
+      <c r="J10" s="61"/>
       <c r="K10" s="41"/>
       <c r="L10" s="41"/>
       <c r="M10" s="3" t="s">
@@ -4019,7 +4074,7 @@
       <c r="Q10" s="5">
         <v>0.69125847064969603</v>
       </c>
-      <c r="S10" s="65"/>
+      <c r="S10" s="61"/>
       <c r="T10" s="41"/>
       <c r="U10" s="41"/>
       <c r="V10" s="3" t="s">
@@ -4039,7 +4094,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="66"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
       <c r="D11" s="6" t="s">
@@ -4057,7 +4112,7 @@
       <c r="H11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="66"/>
+      <c r="J11" s="62"/>
       <c r="K11" s="42"/>
       <c r="L11" s="42"/>
       <c r="M11" s="6" t="s">
@@ -4075,7 +4130,7 @@
       <c r="Q11" s="12">
         <v>5.7849128320341904E-4</v>
       </c>
-      <c r="S11" s="66"/>
+      <c r="S11" s="62"/>
       <c r="T11" s="42"/>
       <c r="U11" s="42"/>
       <c r="V11" s="6" t="s">
@@ -4095,7 +4150,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="43"/>
@@ -4115,7 +4170,7 @@
       <c r="H12" s="26">
         <v>0.80183396861683798</v>
       </c>
-      <c r="J12" s="61" t="s">
+      <c r="J12" s="63" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="43"/>
@@ -4135,7 +4190,7 @@
       <c r="Q12" s="26">
         <v>0.396063757387072</v>
       </c>
-      <c r="S12" s="61" t="s">
+      <c r="S12" s="63" t="s">
         <v>22</v>
       </c>
       <c r="T12" s="43"/>
@@ -4157,7 +4212,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
@@ -4175,7 +4230,7 @@
       <c r="H13" s="15">
         <v>0.81920679808716201</v>
       </c>
-      <c r="J13" s="62"/>
+      <c r="J13" s="64"/>
       <c r="K13" s="44"/>
       <c r="L13" s="44"/>
       <c r="M13" s="13" t="s">
@@ -4193,7 +4248,7 @@
       <c r="Q13" s="15">
         <v>0.47782379499238098</v>
       </c>
-      <c r="S13" s="62"/>
+      <c r="S13" s="64"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
       <c r="V13" s="13" t="s">
@@ -4213,7 +4268,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="44">
         <v>0.46</v>
       </c>
@@ -4235,7 +4290,7 @@
       <c r="H14" s="22">
         <v>1.1522972880144901E-2</v>
       </c>
-      <c r="J14" s="62"/>
+      <c r="J14" s="64"/>
       <c r="K14" s="44">
         <v>0.27</v>
       </c>
@@ -4257,7 +4312,7 @@
       <c r="Q14" s="15">
         <v>0.63983558618550995</v>
       </c>
-      <c r="S14" s="62"/>
+      <c r="S14" s="64"/>
       <c r="T14" s="44">
         <v>0.17</v>
       </c>
@@ -4281,7 +4336,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
       <c r="D15" s="13" t="s">
@@ -4299,7 +4354,7 @@
       <c r="H15" s="15">
         <v>0.71318423509832796</v>
       </c>
-      <c r="J15" s="62"/>
+      <c r="J15" s="64"/>
       <c r="K15" s="44"/>
       <c r="L15" s="44"/>
       <c r="M15" s="13" t="s">
@@ -4317,7 +4372,7 @@
       <c r="Q15" s="15">
         <v>0.12996489935105601</v>
       </c>
-      <c r="S15" s="62"/>
+      <c r="S15" s="64"/>
       <c r="T15" s="44"/>
       <c r="U15" s="44"/>
       <c r="V15" s="13" t="s">
@@ -4337,7 +4392,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="63"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
       <c r="D16" s="16" t="s">
@@ -4355,7 +4410,7 @@
       <c r="H16" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="63"/>
+      <c r="J16" s="65"/>
       <c r="K16" s="45"/>
       <c r="L16" s="45"/>
       <c r="M16" s="16" t="s">
@@ -4373,7 +4428,7 @@
       <c r="Q16" s="19">
         <v>6.4203448897037795E-4</v>
       </c>
-      <c r="S16" s="63"/>
+      <c r="S16" s="65"/>
       <c r="T16" s="45"/>
       <c r="U16" s="45"/>
       <c r="V16" s="16" t="s">
@@ -4393,7 +4448,7 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="60" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="40"/>
@@ -4413,7 +4468,7 @@
       <c r="H17" s="28">
         <v>1.4661160013996999E-2</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="J17" s="60" t="s">
         <v>17</v>
       </c>
       <c r="K17" s="40"/>
@@ -4433,7 +4488,7 @@
       <c r="Q17" s="27">
         <v>0.63226305707268105</v>
       </c>
-      <c r="S17" s="64" t="s">
+      <c r="S17" s="60" t="s">
         <v>23</v>
       </c>
       <c r="T17" s="40"/>
@@ -4455,7 +4510,7 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="3" t="s">
@@ -4473,7 +4528,7 @@
       <c r="H18" s="10">
         <v>1.03589205298071E-4</v>
       </c>
-      <c r="J18" s="65"/>
+      <c r="J18" s="61"/>
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="3" t="s">
@@ -4491,7 +4546,7 @@
       <c r="Q18" s="5">
         <v>0.63091798944421296</v>
       </c>
-      <c r="S18" s="65"/>
+      <c r="S18" s="61"/>
       <c r="T18" s="41"/>
       <c r="U18" s="41"/>
       <c r="V18" s="3" t="s">
@@ -4511,7 +4566,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="41">
         <v>0.37</v>
       </c>
@@ -4533,7 +4588,7 @@
       <c r="H19" s="10">
         <v>3.4893820447861899E-2</v>
       </c>
-      <c r="J19" s="65"/>
+      <c r="J19" s="61"/>
       <c r="K19" s="41">
         <v>0.12</v>
       </c>
@@ -4555,7 +4610,7 @@
       <c r="Q19" s="5">
         <v>0.19006605256154599</v>
       </c>
-      <c r="S19" s="65"/>
+      <c r="S19" s="61"/>
       <c r="T19" s="41">
         <v>0.09</v>
       </c>
@@ -4579,7 +4634,7 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="3" t="s">
@@ -4597,7 +4652,7 @@
       <c r="H20" s="5">
         <v>0.58894272291956795</v>
       </c>
-      <c r="J20" s="65"/>
+      <c r="J20" s="61"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="3" t="s">
@@ -4615,7 +4670,7 @@
       <c r="Q20" s="5">
         <v>0.45770082770904802</v>
       </c>
-      <c r="S20" s="65"/>
+      <c r="S20" s="61"/>
       <c r="T20" s="41"/>
       <c r="U20" s="41"/>
       <c r="V20" s="3" t="s">
@@ -4635,7 +4690,7 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="66"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="6" t="s">
@@ -4653,7 +4708,7 @@
       <c r="H21" s="8">
         <v>8.1306385386086505E-2</v>
       </c>
-      <c r="J21" s="66"/>
+      <c r="J21" s="62"/>
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
       <c r="M21" s="6" t="s">
@@ -4671,7 +4726,7 @@
       <c r="Q21" s="8">
         <v>0.17256483293313099</v>
       </c>
-      <c r="S21" s="66"/>
+      <c r="S21" s="62"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
       <c r="V21" s="6" t="s">
@@ -4691,7 +4746,7 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="63" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="43"/>
@@ -4711,7 +4766,7 @@
       <c r="H22" s="26">
         <v>0.156590362282719</v>
       </c>
-      <c r="J22" s="61" t="s">
+      <c r="J22" s="63" t="s">
         <v>18</v>
       </c>
       <c r="K22" s="43"/>
@@ -4731,7 +4786,7 @@
       <c r="Q22" s="26">
         <v>0.69885942821946401</v>
       </c>
-      <c r="S22" s="61" t="s">
+      <c r="S22" s="63" t="s">
         <v>24</v>
       </c>
       <c r="T22" s="43"/>
@@ -4753,7 +4808,7 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
       <c r="D23" s="13" t="s">
@@ -4771,7 +4826,7 @@
       <c r="H23" s="15">
         <v>0.904389521648304</v>
       </c>
-      <c r="J23" s="62"/>
+      <c r="J23" s="64"/>
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
       <c r="M23" s="13" t="s">
@@ -4789,7 +4844,7 @@
       <c r="Q23" s="15">
         <v>0.62584133799445296</v>
       </c>
-      <c r="S23" s="62"/>
+      <c r="S23" s="64"/>
       <c r="T23" s="44"/>
       <c r="U23" s="44"/>
       <c r="V23" s="13" t="s">
@@ -4809,7 +4864,7 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="44">
         <v>0.1</v>
       </c>
@@ -4831,7 +4886,7 @@
       <c r="H24" s="15">
         <v>0.30569527576697603</v>
       </c>
-      <c r="J24" s="62"/>
+      <c r="J24" s="64"/>
       <c r="K24" s="44">
         <v>0.08</v>
       </c>
@@ -4853,7 +4908,7 @@
       <c r="Q24" s="15">
         <v>0.56359297147337195</v>
       </c>
-      <c r="S24" s="62"/>
+      <c r="S24" s="64"/>
       <c r="T24" s="44">
         <v>0.1</v>
       </c>
@@ -4877,7 +4932,7 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A25" s="62"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="13" t="s">
@@ -4895,7 +4950,7 @@
       <c r="H25" s="15">
         <v>0.68583510960772898</v>
       </c>
-      <c r="J25" s="62"/>
+      <c r="J25" s="64"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="13" t="s">
@@ -4913,7 +4968,7 @@
       <c r="Q25" s="15">
         <v>0.70588105337253604</v>
       </c>
-      <c r="S25" s="62"/>
+      <c r="S25" s="64"/>
       <c r="T25" s="44"/>
       <c r="U25" s="44"/>
       <c r="V25" s="13" t="s">
@@ -4933,7 +4988,7 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
       <c r="D26" s="16" t="s">
@@ -4951,7 +5006,7 @@
       <c r="H26" s="20">
         <v>0.41122866769062399</v>
       </c>
-      <c r="J26" s="63"/>
+      <c r="J26" s="65"/>
       <c r="K26" s="45"/>
       <c r="L26" s="45"/>
       <c r="M26" s="16" t="s">
@@ -4969,7 +5024,7 @@
       <c r="Q26" s="20">
         <v>0.24845922044221999</v>
       </c>
-      <c r="S26" s="63"/>
+      <c r="S26" s="65"/>
       <c r="T26" s="45"/>
       <c r="U26" s="45"/>
       <c r="V26" s="16" t="s">
@@ -4989,7 +5044,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="60" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="40"/>
@@ -5009,7 +5064,7 @@
       <c r="H27" s="28">
         <v>1.02956589885583E-2</v>
       </c>
-      <c r="J27" s="64" t="s">
+      <c r="J27" s="60" t="s">
         <v>19</v>
       </c>
       <c r="K27" s="40"/>
@@ -5029,7 +5084,7 @@
       <c r="Q27" s="27">
         <v>0.91086414946984995</v>
       </c>
-      <c r="S27" s="64" t="s">
+      <c r="S27" s="60" t="s">
         <v>25</v>
       </c>
       <c r="T27" s="40"/>
@@ -5051,7 +5106,7 @@
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
       <c r="D28" s="3" t="s">
@@ -5069,7 +5124,7 @@
       <c r="H28" s="10">
         <v>4.8954711894798199E-2</v>
       </c>
-      <c r="J28" s="65"/>
+      <c r="J28" s="61"/>
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="3" t="s">
@@ -5087,7 +5142,7 @@
       <c r="Q28" s="5">
         <v>0.95282317254778404</v>
       </c>
-      <c r="S28" s="65"/>
+      <c r="S28" s="61"/>
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="V28" s="3" t="s">
@@ -5107,7 +5162,7 @@
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="41">
         <v>0.54</v>
       </c>
@@ -5129,7 +5184,7 @@
       <c r="H29" s="5">
         <v>0.60274047594928004</v>
       </c>
-      <c r="J29" s="65"/>
+      <c r="J29" s="61"/>
       <c r="K29" s="41">
         <v>0.68</v>
       </c>
@@ -5151,7 +5206,7 @@
       <c r="Q29" s="5">
         <v>0.72885199050288396</v>
       </c>
-      <c r="S29" s="65"/>
+      <c r="S29" s="61"/>
       <c r="T29" s="41">
         <v>0.05</v>
       </c>
@@ -5175,7 +5230,7 @@
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
       <c r="D30" s="3" t="s">
@@ -5193,7 +5248,7 @@
       <c r="H30" s="5">
         <v>0.100097196819914</v>
       </c>
-      <c r="J30" s="65"/>
+      <c r="J30" s="61"/>
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="3" t="s">
@@ -5211,7 +5266,7 @@
       <c r="Q30" s="5">
         <v>0.45481679394520702</v>
       </c>
-      <c r="S30" s="65"/>
+      <c r="S30" s="61"/>
       <c r="T30" s="41"/>
       <c r="U30" s="41"/>
       <c r="V30" s="3" t="s">
@@ -5231,7 +5286,7 @@
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A31" s="66"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
       <c r="D31" s="6" t="s">
@@ -5249,7 +5304,7 @@
       <c r="H31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="66"/>
+      <c r="J31" s="62"/>
       <c r="K31" s="42"/>
       <c r="L31" s="42"/>
       <c r="M31" s="6" t="s">
@@ -5267,7 +5322,7 @@
       <c r="Q31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="S31" s="66"/>
+      <c r="S31" s="62"/>
       <c r="T31" s="42"/>
       <c r="U31" s="42"/>
       <c r="V31" s="6" t="s">
@@ -5288,12 +5343,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
     <mergeCell ref="S27:S31"/>
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="J7:J11"/>
@@ -5306,6 +5355,12 @@
     <mergeCell ref="S12:S16"/>
     <mergeCell ref="S17:S21"/>
     <mergeCell ref="S22:S26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5316,7 +5371,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5340,10 +5395,10 @@
       <c r="E1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="58" t="s">
         <v>92</v>
       </c>
     </row>
@@ -5366,7 +5421,7 @@
       <c r="G2" s="14">
         <v>0.43</v>
       </c>
-      <c r="H2" s="67">
+      <c r="H2" s="59">
         <v>0.76</v>
       </c>
     </row>
@@ -5464,7 +5519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA57C79B-597D-4C75-A549-1798BCB1BB79}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -5489,10 +5544,10 @@
       <c r="E1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="58" t="s">
         <v>92</v>
       </c>
     </row>
@@ -5512,10 +5567,10 @@
       <c r="E2" s="22">
         <v>2.7687839999999998E-2</v>
       </c>
-      <c r="G2" s="67">
+      <c r="G2" s="59">
         <v>0.27</v>
       </c>
-      <c r="H2" s="67">
+      <c r="H2" s="59">
         <v>0.82</v>
       </c>
     </row>
@@ -5607,4 +5662,303 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D9F11B-EFAD-4DF3-B541-EC1B3775B03E}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="66">
+        <v>0.02</v>
+      </c>
+      <c r="C2" s="66">
+        <v>0.13</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="67">
+        <v>-0.69682290000000002</v>
+      </c>
+      <c r="F2" s="68">
+        <v>0.26659928999999999</v>
+      </c>
+      <c r="G2" s="68">
+        <v>-2.6137459999999999</v>
+      </c>
+      <c r="H2" s="69">
+        <v>8.9555539999999993E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="71">
+        <v>-0.8702917</v>
+      </c>
+      <c r="F3" s="72">
+        <v>0.26659928999999999</v>
+      </c>
+      <c r="G3" s="72">
+        <v>-3.2644190000000002</v>
+      </c>
+      <c r="H3" s="73">
+        <v>1.0968900000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="75">
+        <v>0.01</v>
+      </c>
+      <c r="C4" s="75">
+        <v>0.42</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="76">
+        <v>0.39358779999999999</v>
+      </c>
+      <c r="F4" s="76">
+        <v>0.25136041999999997</v>
+      </c>
+      <c r="G4" s="76">
+        <v>1.5658300000000001</v>
+      </c>
+      <c r="H4" s="77">
+        <v>0.1173884</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="85">
+        <v>-1.0091218</v>
+      </c>
+      <c r="F5" s="79">
+        <v>0.25136041999999997</v>
+      </c>
+      <c r="G5" s="79">
+        <v>-4.0146410000000001</v>
+      </c>
+      <c r="H5" s="84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="66">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="67">
+        <v>4.4245760000000001</v>
+      </c>
+      <c r="F6" s="68">
+        <v>0.53118730000000003</v>
+      </c>
+      <c r="G6" s="68">
+        <v>8.3295960000000004</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="81"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="71">
+        <v>-1.7969949999999999</v>
+      </c>
+      <c r="F7" s="72">
+        <v>0.53118730000000003</v>
+      </c>
+      <c r="G7" s="72">
+        <v>-3.382978</v>
+      </c>
+      <c r="H7" s="73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="75">
+        <v>0.03</v>
+      </c>
+      <c r="C8" s="75">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="76">
+        <v>-0.37195499999999998</v>
+      </c>
+      <c r="F8" s="76">
+        <v>0.23623229000000001</v>
+      </c>
+      <c r="G8" s="76">
+        <v>-1.5745309999999999</v>
+      </c>
+      <c r="H8" s="77">
+        <v>0.1153648</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="83"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="85">
+        <v>-1.0671889999999999</v>
+      </c>
+      <c r="F9" s="79">
+        <v>0.23623229000000001</v>
+      </c>
+      <c r="G9" s="79">
+        <v>-4.5175390000000002</v>
+      </c>
+      <c r="H9" s="84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="66">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="66">
+        <v>0.08</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="68">
+        <v>-0.1822646</v>
+      </c>
+      <c r="F10" s="68">
+        <v>0.28269546000000001</v>
+      </c>
+      <c r="G10" s="68">
+        <v>-0.64473840000000004</v>
+      </c>
+      <c r="H10" s="74">
+        <v>0.51909673099999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="71">
+        <v>-0.7442782</v>
+      </c>
+      <c r="F11" s="72">
+        <v>0.28269546000000001</v>
+      </c>
+      <c r="G11" s="72">
+        <v>-2.6327913999999999</v>
+      </c>
+      <c r="H11" s="73">
+        <v>8.4686339999999992E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
removing unused files, correcting error where soil P was replaced with soil Ca, adding partial effects to individual nutrient plots
</commit_message>
<xml_diff>
--- a/outputs/SupplementalTables.xlsx
+++ b/outputs/SupplementalTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\AppraisingGrazing\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332137AB-E140-480A-BE66-7525C6A350B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D225CF-D855-42FD-9DDB-AA0E5E85A297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="6" xr2:uid="{CF962987-2438-4E1C-BBD3-768B42620E9E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="1" xr2:uid="{CF962987-2438-4E1C-BBD3-768B42620E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="SiteDescriptions" sheetId="5" r:id="rId1"/>
@@ -593,7 +593,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -798,6 +798,55 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -822,6 +871,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -834,83 +889,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1730,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9345813A-2DFE-4E66-B055-012251326829}">
   <dimension ref="A1:AF36"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Q1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1824,7 +1803,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="92" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="44"/>
@@ -1844,7 +1823,7 @@
       <c r="H2" s="15">
         <v>0.75643309065928399</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="92" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="44"/>
@@ -1864,7 +1843,7 @@
       <c r="Q2" s="15">
         <v>0.78445569199090504</v>
       </c>
-      <c r="S2" s="75" t="s">
+      <c r="S2" s="92" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="44"/>
@@ -1886,7 +1865,7 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="76"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
       <c r="D3" s="13" t="s">
@@ -1904,7 +1883,7 @@
       <c r="H3" s="15">
         <v>0.85620580622572096</v>
       </c>
-      <c r="J3" s="76"/>
+      <c r="J3" s="93"/>
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
       <c r="M3" s="13" t="s">
@@ -1922,7 +1901,7 @@
       <c r="Q3" s="15">
         <v>0.111358770556964</v>
       </c>
-      <c r="S3" s="76"/>
+      <c r="S3" s="93"/>
       <c r="T3" s="44"/>
       <c r="U3" s="44"/>
       <c r="V3" s="13" t="s">
@@ -1942,7 +1921,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="44">
         <v>0.59</v>
       </c>
@@ -1964,7 +1943,7 @@
       <c r="H4" s="15">
         <v>0.198730750798048</v>
       </c>
-      <c r="J4" s="76"/>
+      <c r="J4" s="93"/>
       <c r="K4" s="44">
         <v>0.41</v>
       </c>
@@ -1986,7 +1965,7 @@
       <c r="Q4" s="15">
         <v>0.54152757122083806</v>
       </c>
-      <c r="S4" s="76"/>
+      <c r="S4" s="93"/>
       <c r="T4" s="44">
         <v>0.21</v>
       </c>
@@ -2010,7 +1989,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="76"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="13" t="s">
@@ -2028,7 +2007,7 @@
       <c r="H5" s="22">
         <v>2.0426214511249902E-2</v>
       </c>
-      <c r="J5" s="76"/>
+      <c r="J5" s="93"/>
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
       <c r="M5" s="13" t="s">
@@ -2046,7 +2025,7 @@
       <c r="Q5" s="15">
         <v>0.58620851191461298</v>
       </c>
-      <c r="S5" s="76"/>
+      <c r="S5" s="93"/>
       <c r="T5" s="44"/>
       <c r="U5" s="44"/>
       <c r="V5" s="13" t="s">
@@ -2066,7 +2045,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="77"/>
+      <c r="A6" s="94"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
       <c r="D6" s="16" t="s">
@@ -2084,7 +2063,7 @@
       <c r="H6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="77"/>
+      <c r="J6" s="94"/>
       <c r="K6" s="45"/>
       <c r="L6" s="45"/>
       <c r="M6" s="16" t="s">
@@ -2102,7 +2081,7 @@
       <c r="Q6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="77"/>
+      <c r="S6" s="94"/>
       <c r="T6" s="45"/>
       <c r="U6" s="45"/>
       <c r="V6" s="16" t="s">
@@ -2122,7 +2101,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="89" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="41"/>
@@ -2142,7 +2121,7 @@
       <c r="H7" s="5">
         <v>0.45450659664544801</v>
       </c>
-      <c r="J7" s="72" t="s">
+      <c r="J7" s="89" t="s">
         <v>13</v>
       </c>
       <c r="K7" s="41"/>
@@ -2162,7 +2141,7 @@
       <c r="Q7" s="5">
         <v>0.96017688602466</v>
       </c>
-      <c r="S7" s="72" t="s">
+      <c r="S7" s="89" t="s">
         <v>19</v>
       </c>
       <c r="T7" s="41"/>
@@ -2184,7 +2163,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="73"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="3" t="s">
@@ -2202,7 +2181,7 @@
       <c r="H8" s="5">
         <v>0.53062471950727597</v>
       </c>
-      <c r="J8" s="73"/>
+      <c r="J8" s="90"/>
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="3" t="s">
@@ -2220,7 +2199,7 @@
       <c r="Q8" s="5">
         <v>0.49430589283329901</v>
       </c>
-      <c r="S8" s="73"/>
+      <c r="S8" s="90"/>
       <c r="T8" s="41"/>
       <c r="U8" s="41"/>
       <c r="V8" s="3" t="s">
@@ -2240,7 +2219,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="73"/>
+      <c r="A9" s="90"/>
       <c r="B9" s="41">
         <v>0.23</v>
       </c>
@@ -2262,7 +2241,7 @@
       <c r="H9" s="5">
         <v>0.85845654845826103</v>
       </c>
-      <c r="J9" s="73"/>
+      <c r="J9" s="90"/>
       <c r="K9" s="41">
         <v>0.32</v>
       </c>
@@ -2284,7 +2263,7 @@
       <c r="Q9" s="5">
         <v>0.12333957548581399</v>
       </c>
-      <c r="S9" s="73"/>
+      <c r="S9" s="90"/>
       <c r="T9" s="41">
         <v>0.21</v>
       </c>
@@ -2308,7 +2287,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="73"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="3" t="s">
@@ -2326,7 +2305,7 @@
       <c r="H10" s="5">
         <v>0.68725480675239803</v>
       </c>
-      <c r="J10" s="73"/>
+      <c r="J10" s="90"/>
       <c r="K10" s="41"/>
       <c r="L10" s="41"/>
       <c r="M10" s="3" t="s">
@@ -2344,7 +2323,7 @@
       <c r="Q10" s="5">
         <v>0.56468785934212196</v>
       </c>
-      <c r="S10" s="73"/>
+      <c r="S10" s="90"/>
       <c r="T10" s="41"/>
       <c r="U10" s="41"/>
       <c r="V10" s="3" t="s">
@@ -2364,7 +2343,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
       <c r="D11" s="6" t="s">
@@ -2382,7 +2361,7 @@
       <c r="H11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="74"/>
+      <c r="J11" s="91"/>
       <c r="K11" s="42"/>
       <c r="L11" s="42"/>
       <c r="M11" s="6" t="s">
@@ -2400,7 +2379,7 @@
       <c r="Q11" s="12">
         <v>5.6703110896494401E-4</v>
       </c>
-      <c r="S11" s="74"/>
+      <c r="S11" s="91"/>
       <c r="T11" s="42"/>
       <c r="U11" s="42"/>
       <c r="V11" s="6" t="s">
@@ -2421,7 +2400,7 @@
       <c r="AF11" s="35"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="92" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="44"/>
@@ -2441,7 +2420,7 @@
       <c r="H12" s="15">
         <v>0.70634877764113901</v>
       </c>
-      <c r="J12" s="75" t="s">
+      <c r="J12" s="92" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="44"/>
@@ -2461,7 +2440,7 @@
       <c r="Q12" s="15">
         <v>0.96903819673954605</v>
       </c>
-      <c r="S12" s="75" t="s">
+      <c r="S12" s="92" t="s">
         <v>20</v>
       </c>
       <c r="T12" s="44"/>
@@ -2470,20 +2449,20 @@
         <v>0</v>
       </c>
       <c r="W12" s="14">
-        <v>8.9411824277785101E-2</v>
+        <v>-6.8683749960923995E-2</v>
       </c>
       <c r="X12" s="14">
-        <v>0.127158985954198</v>
+        <v>0.13406651483597801</v>
       </c>
       <c r="Y12" s="14">
-        <v>0.70314986870051799</v>
+        <v>-0.51231099760409304</v>
       </c>
       <c r="Z12" s="15">
-        <v>0.48196235697490403</v>
+        <v>0.60843336958759897</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="76"/>
+      <c r="A13" s="93"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
@@ -2501,7 +2480,7 @@
       <c r="H13" s="15">
         <v>0.98064258715030805</v>
       </c>
-      <c r="J13" s="76"/>
+      <c r="J13" s="93"/>
       <c r="K13" s="44"/>
       <c r="L13" s="44"/>
       <c r="M13" s="13" t="s">
@@ -2519,27 +2498,27 @@
       <c r="Q13" s="15">
         <v>0.204959108693586</v>
       </c>
-      <c r="S13" s="76"/>
+      <c r="S13" s="93"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
       <c r="V13" s="13" t="s">
         <v>1</v>
       </c>
       <c r="W13" s="14">
-        <v>-7.5774502890207096E-2</v>
+        <v>-0.13339475217539901</v>
       </c>
       <c r="X13" s="14">
-        <v>0.127158985954198</v>
+        <v>0.13406651483597801</v>
       </c>
       <c r="Y13" s="14">
-        <v>-0.595903642370196</v>
+        <v>-0.99498933300830905</v>
       </c>
       <c r="Z13" s="15">
-        <v>0.55123959982481097</v>
+        <v>0.31974145238871698</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="76"/>
+      <c r="A14" s="93"/>
       <c r="B14" s="44">
         <v>0.36</v>
       </c>
@@ -2561,7 +2540,7 @@
       <c r="H14" s="15">
         <v>0.46443467686441597</v>
       </c>
-      <c r="J14" s="76"/>
+      <c r="J14" s="93"/>
       <c r="K14" s="44">
         <v>0.33</v>
       </c>
@@ -2583,7 +2562,7 @@
       <c r="Q14" s="15">
         <v>0.28711644693738703</v>
       </c>
-      <c r="S14" s="76"/>
+      <c r="S14" s="93"/>
       <c r="T14" s="44">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2594,20 +2573,20 @@
         <v>31</v>
       </c>
       <c r="W14" s="14">
-        <v>-7.3413121855626595E-2</v>
+        <v>0.17431841062523301</v>
       </c>
       <c r="X14" s="14">
-        <v>0.127158985954198</v>
+        <v>0.13406651483597801</v>
       </c>
       <c r="Y14" s="14">
-        <v>-0.57733333829879496</v>
+        <v>1.3002382499351199</v>
       </c>
       <c r="Z14" s="15">
-        <v>0.56371429674058304</v>
+        <v>0.193519324704434</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="76"/>
+      <c r="A15" s="93"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
       <c r="D15" s="13" t="s">
@@ -2625,7 +2604,7 @@
       <c r="H15" s="15">
         <v>0.17886255886840399</v>
       </c>
-      <c r="J15" s="76"/>
+      <c r="J15" s="93"/>
       <c r="K15" s="44"/>
       <c r="L15" s="44"/>
       <c r="M15" s="13" t="s">
@@ -2643,27 +2622,27 @@
       <c r="Q15" s="15">
         <v>0.43957422325523998</v>
       </c>
-      <c r="S15" s="76"/>
+      <c r="S15" s="93"/>
       <c r="T15" s="44"/>
       <c r="U15" s="44"/>
       <c r="V15" s="13" t="s">
         <v>32</v>
       </c>
       <c r="W15" s="14">
-        <v>5.0931924485710697E-2</v>
+        <v>1.6554583521734601E-2</v>
       </c>
       <c r="X15" s="14">
-        <v>0.127158985954198</v>
+        <v>0.13406651483597801</v>
       </c>
       <c r="Y15" s="14">
-        <v>0.40053735961732301</v>
+        <v>0.123480374961549</v>
       </c>
       <c r="Z15" s="15">
-        <v>0.68876077232800903</v>
+        <v>0.90172671386593595</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" s="77"/>
+      <c r="A16" s="94"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
       <c r="D16" s="16" t="s">
@@ -2681,7 +2660,7 @@
       <c r="H16" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="77"/>
+      <c r="J16" s="94"/>
       <c r="K16" s="45"/>
       <c r="L16" s="45"/>
       <c r="M16" s="16" t="s">
@@ -2699,28 +2678,27 @@
       <c r="Q16" s="19">
         <v>9.5878767935397803E-4</v>
       </c>
-      <c r="S16" s="77"/>
+      <c r="S16" s="94"/>
       <c r="T16" s="45"/>
       <c r="U16" s="45"/>
       <c r="V16" s="16" t="s">
         <v>26</v>
       </c>
       <c r="W16" s="18">
-        <v>6.2220215512979703E-3</v>
+        <v>7.8552265845189595E-2</v>
       </c>
       <c r="X16" s="18">
-        <v>2.6301465255499701E-2</v>
+        <v>3.7919736708226903E-2</v>
       </c>
       <c r="Y16" s="18">
-        <v>0.236565586398154</v>
+        <v>2.0715403814538398</v>
       </c>
       <c r="Z16" s="20">
-        <v>0.81299382050265701</v>
-      </c>
-      <c r="AF16" s="35"/>
+        <v>3.8308324805831101E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="89" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="41"/>
@@ -2740,7 +2718,7 @@
       <c r="H17" s="10">
         <v>4.2440815812778497E-2</v>
       </c>
-      <c r="J17" s="72" t="s">
+      <c r="J17" s="89" t="s">
         <v>15</v>
       </c>
       <c r="K17" s="41"/>
@@ -2760,7 +2738,7 @@
       <c r="Q17" s="5">
         <v>0.50381674695789302</v>
       </c>
-      <c r="S17" s="72" t="s">
+      <c r="S17" s="89" t="s">
         <v>21</v>
       </c>
       <c r="T17" s="41"/>
@@ -2782,7 +2760,7 @@
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A18" s="73"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="3" t="s">
@@ -2800,7 +2778,7 @@
       <c r="H18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="73"/>
+      <c r="J18" s="90"/>
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="3" t="s">
@@ -2818,7 +2796,7 @@
       <c r="Q18" s="5">
         <v>0.264487950777611</v>
       </c>
-      <c r="S18" s="73"/>
+      <c r="S18" s="90"/>
       <c r="T18" s="41"/>
       <c r="U18" s="41"/>
       <c r="V18" s="3" t="s">
@@ -2838,7 +2816,7 @@
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A19" s="73"/>
+      <c r="A19" s="90"/>
       <c r="B19" s="41">
         <v>0.31</v>
       </c>
@@ -2860,7 +2838,7 @@
       <c r="H19" s="5">
         <v>9.6818088993625706E-2</v>
       </c>
-      <c r="J19" s="73"/>
+      <c r="J19" s="90"/>
       <c r="K19" s="41">
         <v>0.26</v>
       </c>
@@ -2882,7 +2860,7 @@
       <c r="Q19" s="5">
         <v>0.37610715062244399</v>
       </c>
-      <c r="S19" s="73"/>
+      <c r="S19" s="90"/>
       <c r="T19" s="41">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2906,7 +2884,7 @@
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A20" s="73"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="3" t="s">
@@ -2924,7 +2902,7 @@
       <c r="H20" s="10">
         <v>6.5707623725130805E-4</v>
       </c>
-      <c r="J20" s="73"/>
+      <c r="J20" s="90"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="3" t="s">
@@ -2942,7 +2920,7 @@
       <c r="Q20" s="5">
         <v>0.239285481771352</v>
       </c>
-      <c r="S20" s="73"/>
+      <c r="S20" s="90"/>
       <c r="T20" s="41"/>
       <c r="U20" s="41"/>
       <c r="V20" s="3" t="s">
@@ -2962,7 +2940,7 @@
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A21" s="74"/>
+      <c r="A21" s="91"/>
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="6" t="s">
@@ -2980,7 +2958,7 @@
       <c r="H21" s="12">
         <v>5.7643528578590598E-2</v>
       </c>
-      <c r="J21" s="74"/>
+      <c r="J21" s="91"/>
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
       <c r="M21" s="6" t="s">
@@ -2998,7 +2976,7 @@
       <c r="Q21" s="8">
         <v>0.18897297602503599</v>
       </c>
-      <c r="S21" s="74"/>
+      <c r="S21" s="91"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
       <c r="V21" s="6" t="s">
@@ -3018,7 +2996,7 @@
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="92" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="44"/>
@@ -3038,7 +3016,7 @@
       <c r="H22" s="15">
         <v>5.8951439115694199E-2</v>
       </c>
-      <c r="J22" s="75" t="s">
+      <c r="J22" s="92" t="s">
         <v>16</v>
       </c>
       <c r="K22" s="44"/>
@@ -3058,7 +3036,7 @@
       <c r="Q22" s="15">
         <v>0.85580186913876699</v>
       </c>
-      <c r="S22" s="75" t="s">
+      <c r="S22" s="92" t="s">
         <v>22</v>
       </c>
       <c r="T22" s="44"/>
@@ -3080,7 +3058,7 @@
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A23" s="76"/>
+      <c r="A23" s="93"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
       <c r="D23" s="13" t="s">
@@ -3098,7 +3076,7 @@
       <c r="H23" s="15">
         <v>0.898896282859034</v>
       </c>
-      <c r="J23" s="76"/>
+      <c r="J23" s="93"/>
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
       <c r="M23" s="13" t="s">
@@ -3116,7 +3094,7 @@
       <c r="Q23" s="15">
         <v>0.53963880509304496</v>
       </c>
-      <c r="S23" s="76"/>
+      <c r="S23" s="93"/>
       <c r="T23" s="44"/>
       <c r="U23" s="44"/>
       <c r="V23" s="13" t="s">
@@ -3136,7 +3114,7 @@
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A24" s="76"/>
+      <c r="A24" s="93"/>
       <c r="B24" s="44">
         <v>0.13</v>
       </c>
@@ -3158,7 +3136,7 @@
       <c r="H24" s="15">
         <v>0.56247855473640496</v>
       </c>
-      <c r="J24" s="76"/>
+      <c r="J24" s="93"/>
       <c r="K24" s="44">
         <v>0.27</v>
       </c>
@@ -3180,7 +3158,7 @@
       <c r="Q24" s="15">
         <v>0.19620110579128799</v>
       </c>
-      <c r="S24" s="76"/>
+      <c r="S24" s="93"/>
       <c r="T24" s="44">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -3204,7 +3182,7 @@
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A25" s="76"/>
+      <c r="A25" s="93"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="13" t="s">
@@ -3222,7 +3200,7 @@
       <c r="H25" s="15">
         <v>0.96061530261722605</v>
       </c>
-      <c r="J25" s="76"/>
+      <c r="J25" s="93"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="13" t="s">
@@ -3240,7 +3218,7 @@
       <c r="Q25" s="15">
         <v>0.57714986420537495</v>
       </c>
-      <c r="S25" s="76"/>
+      <c r="S25" s="93"/>
       <c r="T25" s="44"/>
       <c r="U25" s="44"/>
       <c r="V25" s="13" t="s">
@@ -3260,7 +3238,7 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A26" s="77"/>
+      <c r="A26" s="94"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
       <c r="D26" s="16" t="s">
@@ -3278,7 +3256,7 @@
       <c r="H26" s="20">
         <v>0.32774660012482898</v>
       </c>
-      <c r="J26" s="77"/>
+      <c r="J26" s="94"/>
       <c r="K26" s="45"/>
       <c r="L26" s="45"/>
       <c r="M26" s="16" t="s">
@@ -3296,7 +3274,7 @@
       <c r="Q26" s="20">
         <v>0.21330625309083201</v>
       </c>
-      <c r="S26" s="77"/>
+      <c r="S26" s="94"/>
       <c r="T26" s="45"/>
       <c r="U26" s="45"/>
       <c r="V26" s="16" t="s">
@@ -3316,7 +3294,7 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="89" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="41"/>
@@ -3336,7 +3314,7 @@
       <c r="H27" s="10">
         <v>4.0137352839097598E-2</v>
       </c>
-      <c r="J27" s="72" t="s">
+      <c r="J27" s="89" t="s">
         <v>17</v>
       </c>
       <c r="K27" s="41"/>
@@ -3356,7 +3334,7 @@
       <c r="Q27" s="5">
         <v>0.65952820034885495</v>
       </c>
-      <c r="S27" s="72" t="s">
+      <c r="S27" s="89" t="s">
         <v>23</v>
       </c>
       <c r="T27" s="41"/>
@@ -3378,7 +3356,7 @@
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A28" s="73"/>
+      <c r="A28" s="90"/>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
       <c r="D28" s="3" t="s">
@@ -3396,7 +3374,7 @@
       <c r="H28" s="10">
         <v>3.5068868917491801E-2</v>
       </c>
-      <c r="J28" s="73"/>
+      <c r="J28" s="90"/>
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="3" t="s">
@@ -3414,7 +3392,7 @@
       <c r="Q28" s="5">
         <v>0.94359388051558002</v>
       </c>
-      <c r="S28" s="73"/>
+      <c r="S28" s="90"/>
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="V28" s="3" t="s">
@@ -3434,7 +3412,7 @@
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A29" s="73"/>
+      <c r="A29" s="90"/>
       <c r="B29" s="41">
         <v>0.71</v>
       </c>
@@ -3456,7 +3434,7 @@
       <c r="H29" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J29" s="73"/>
+      <c r="J29" s="90"/>
       <c r="K29" s="41">
         <v>0.68</v>
       </c>
@@ -3478,7 +3456,7 @@
       <c r="Q29" s="5">
         <v>0.96316540129969996</v>
       </c>
-      <c r="S29" s="73"/>
+      <c r="S29" s="90"/>
       <c r="T29" s="41">
         <v>0.05</v>
       </c>
@@ -3503,7 +3481,7 @@
       <c r="AF29" s="35"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A30" s="73"/>
+      <c r="A30" s="90"/>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
       <c r="D30" s="3" t="s">
@@ -3521,7 +3499,7 @@
       <c r="H30" s="5">
         <v>7.7615500578327001E-2</v>
       </c>
-      <c r="J30" s="73"/>
+      <c r="J30" s="90"/>
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="3" t="s">
@@ -3539,7 +3517,7 @@
       <c r="Q30" s="5">
         <v>0.83562337156051503</v>
       </c>
-      <c r="S30" s="73"/>
+      <c r="S30" s="90"/>
       <c r="T30" s="41"/>
       <c r="U30" s="41"/>
       <c r="V30" s="3" t="s">
@@ -3559,7 +3537,7 @@
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A31" s="74"/>
+      <c r="A31" s="91"/>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
       <c r="D31" s="6" t="s">
@@ -3577,7 +3555,7 @@
       <c r="H31" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="74"/>
+      <c r="J31" s="91"/>
       <c r="K31" s="42"/>
       <c r="L31" s="42"/>
       <c r="M31" s="6" t="s">
@@ -3595,7 +3573,7 @@
       <c r="Q31" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="S31" s="74"/>
+      <c r="S31" s="91"/>
       <c r="T31" s="42"/>
       <c r="U31" s="42"/>
       <c r="V31" s="6" t="s">
@@ -3620,12 +3598,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
     <mergeCell ref="S27:S31"/>
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="J7:J11"/>
@@ -3638,6 +3610,12 @@
     <mergeCell ref="S12:S16"/>
     <mergeCell ref="S17:S21"/>
     <mergeCell ref="S22:S26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3739,7 +3717,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="92" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="44"/>
@@ -3759,7 +3737,7 @@
       <c r="H2" s="26">
         <v>0.232594480943555</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="92" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="43"/>
@@ -3779,7 +3757,7 @@
       <c r="Q2" s="26">
         <v>0.58051575449478299</v>
       </c>
-      <c r="S2" s="75" t="s">
+      <c r="S2" s="92" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="43"/>
@@ -3801,7 +3779,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="76"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
       <c r="D3" s="13" t="s">
@@ -3819,7 +3797,7 @@
       <c r="H3" s="15">
         <v>0.72085458380743095</v>
       </c>
-      <c r="J3" s="76"/>
+      <c r="J3" s="93"/>
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
       <c r="M3" s="13" t="s">
@@ -3837,7 +3815,7 @@
       <c r="Q3" s="15">
         <v>0.22034570029552</v>
       </c>
-      <c r="S3" s="76"/>
+      <c r="S3" s="93"/>
       <c r="T3" s="44"/>
       <c r="U3" s="44"/>
       <c r="V3" s="13" t="s">
@@ -3857,7 +3835,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="44">
         <v>0.7</v>
       </c>
@@ -3879,7 +3857,7 @@
       <c r="H4" s="22">
         <v>1.62257649215358E-3</v>
       </c>
-      <c r="J4" s="76"/>
+      <c r="J4" s="93"/>
       <c r="K4" s="44">
         <v>0.41</v>
       </c>
@@ -3901,7 +3879,7 @@
       <c r="Q4" s="15">
         <v>0.45992161771271001</v>
       </c>
-      <c r="S4" s="76"/>
+      <c r="S4" s="93"/>
       <c r="T4" s="44">
         <v>0.44</v>
       </c>
@@ -3925,7 +3903,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" s="76"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="13" t="s">
@@ -3943,7 +3921,7 @@
       <c r="H5" s="15">
         <v>0.90736653483351304</v>
       </c>
-      <c r="J5" s="76"/>
+      <c r="J5" s="93"/>
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
       <c r="M5" s="13" t="s">
@@ -3961,7 +3939,7 @@
       <c r="Q5" s="15">
         <v>0.49155219186801202</v>
       </c>
-      <c r="S5" s="76"/>
+      <c r="S5" s="93"/>
       <c r="T5" s="44"/>
       <c r="U5" s="44"/>
       <c r="V5" s="13" t="s">
@@ -3981,7 +3959,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="77"/>
+      <c r="A6" s="94"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
       <c r="D6" s="16" t="s">
@@ -3999,7 +3977,7 @@
       <c r="H6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="77"/>
+      <c r="J6" s="94"/>
       <c r="K6" s="45"/>
       <c r="L6" s="45"/>
       <c r="M6" s="16" t="s">
@@ -4017,7 +3995,7 @@
       <c r="Q6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="77"/>
+      <c r="S6" s="94"/>
       <c r="T6" s="45"/>
       <c r="U6" s="45"/>
       <c r="V6" s="16" t="s">
@@ -4037,7 +4015,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="89" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="41"/>
@@ -4057,7 +4035,7 @@
       <c r="H7" s="27">
         <v>0.552259009406043</v>
       </c>
-      <c r="J7" s="72" t="s">
+      <c r="J7" s="89" t="s">
         <v>13</v>
       </c>
       <c r="K7" s="40"/>
@@ -4077,7 +4055,7 @@
       <c r="Q7" s="27">
         <v>0.32181313500870801</v>
       </c>
-      <c r="S7" s="72" t="s">
+      <c r="S7" s="89" t="s">
         <v>19</v>
       </c>
       <c r="T7" s="40"/>
@@ -4099,7 +4077,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="73"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="3" t="s">
@@ -4117,7 +4095,7 @@
       <c r="H8" s="5">
         <v>0.32335190904313799</v>
       </c>
-      <c r="J8" s="73"/>
+      <c r="J8" s="90"/>
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="3" t="s">
@@ -4135,7 +4113,7 @@
       <c r="Q8" s="5">
         <v>0.85330548504150305</v>
       </c>
-      <c r="S8" s="73"/>
+      <c r="S8" s="90"/>
       <c r="T8" s="41"/>
       <c r="U8" s="41"/>
       <c r="V8" s="3" t="s">
@@ -4155,7 +4133,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" s="73"/>
+      <c r="A9" s="90"/>
       <c r="B9" s="41">
         <v>0.39</v>
       </c>
@@ -4177,7 +4155,7 @@
       <c r="H9" s="5">
         <v>0.124419258908589</v>
       </c>
-      <c r="J9" s="73"/>
+      <c r="J9" s="90"/>
       <c r="K9" s="41">
         <v>0.2</v>
       </c>
@@ -4199,7 +4177,7 @@
       <c r="Q9" s="5">
         <v>0.46405023322165001</v>
       </c>
-      <c r="S9" s="73"/>
+      <c r="S9" s="90"/>
       <c r="T9" s="41">
         <v>0.46</v>
       </c>
@@ -4223,7 +4201,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" s="73"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="3" t="s">
@@ -4241,7 +4219,7 @@
       <c r="H10" s="5">
         <v>0.65137158175371701</v>
       </c>
-      <c r="J10" s="73"/>
+      <c r="J10" s="90"/>
       <c r="K10" s="41"/>
       <c r="L10" s="41"/>
       <c r="M10" s="3" t="s">
@@ -4259,7 +4237,7 @@
       <c r="Q10" s="5">
         <v>0.69125847064969603</v>
       </c>
-      <c r="S10" s="73"/>
+      <c r="S10" s="90"/>
       <c r="T10" s="41"/>
       <c r="U10" s="41"/>
       <c r="V10" s="3" t="s">
@@ -4279,7 +4257,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
       <c r="D11" s="6" t="s">
@@ -4297,7 +4275,7 @@
       <c r="H11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="74"/>
+      <c r="J11" s="91"/>
       <c r="K11" s="42"/>
       <c r="L11" s="42"/>
       <c r="M11" s="6" t="s">
@@ -4315,7 +4293,7 @@
       <c r="Q11" s="12">
         <v>5.7849128320341904E-4</v>
       </c>
-      <c r="S11" s="74"/>
+      <c r="S11" s="91"/>
       <c r="T11" s="42"/>
       <c r="U11" s="42"/>
       <c r="V11" s="6" t="s">
@@ -4335,7 +4313,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="92" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="43"/>
@@ -4355,7 +4333,7 @@
       <c r="H12" s="26">
         <v>0.80183396861683798</v>
       </c>
-      <c r="J12" s="75" t="s">
+      <c r="J12" s="92" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="43"/>
@@ -4375,7 +4353,7 @@
       <c r="Q12" s="26">
         <v>0.396063757387072</v>
       </c>
-      <c r="S12" s="75" t="s">
+      <c r="S12" s="92" t="s">
         <v>20</v>
       </c>
       <c r="T12" s="43"/>
@@ -4397,7 +4375,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="76"/>
+      <c r="A13" s="93"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
@@ -4415,7 +4393,7 @@
       <c r="H13" s="15">
         <v>0.81920679808716201</v>
       </c>
-      <c r="J13" s="76"/>
+      <c r="J13" s="93"/>
       <c r="K13" s="44"/>
       <c r="L13" s="44"/>
       <c r="M13" s="13" t="s">
@@ -4433,7 +4411,7 @@
       <c r="Q13" s="15">
         <v>0.47782379499238098</v>
       </c>
-      <c r="S13" s="76"/>
+      <c r="S13" s="93"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
       <c r="V13" s="13" t="s">
@@ -4453,7 +4431,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="76"/>
+      <c r="A14" s="93"/>
       <c r="B14" s="44">
         <v>0.46</v>
       </c>
@@ -4475,7 +4453,7 @@
       <c r="H14" s="22">
         <v>1.1522972880144901E-2</v>
       </c>
-      <c r="J14" s="76"/>
+      <c r="J14" s="93"/>
       <c r="K14" s="44">
         <v>0.27</v>
       </c>
@@ -4497,7 +4475,7 @@
       <c r="Q14" s="15">
         <v>0.63983558618550995</v>
       </c>
-      <c r="S14" s="76"/>
+      <c r="S14" s="93"/>
       <c r="T14" s="44">
         <v>0.17</v>
       </c>
@@ -4521,7 +4499,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="76"/>
+      <c r="A15" s="93"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
       <c r="D15" s="13" t="s">
@@ -4539,7 +4517,7 @@
       <c r="H15" s="15">
         <v>0.71318423509832796</v>
       </c>
-      <c r="J15" s="76"/>
+      <c r="J15" s="93"/>
       <c r="K15" s="44"/>
       <c r="L15" s="44"/>
       <c r="M15" s="13" t="s">
@@ -4557,7 +4535,7 @@
       <c r="Q15" s="15">
         <v>0.12996489935105601</v>
       </c>
-      <c r="S15" s="76"/>
+      <c r="S15" s="93"/>
       <c r="T15" s="44"/>
       <c r="U15" s="44"/>
       <c r="V15" s="13" t="s">
@@ -4577,7 +4555,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="77"/>
+      <c r="A16" s="94"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
       <c r="D16" s="16" t="s">
@@ -4595,7 +4573,7 @@
       <c r="H16" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="77"/>
+      <c r="J16" s="94"/>
       <c r="K16" s="45"/>
       <c r="L16" s="45"/>
       <c r="M16" s="16" t="s">
@@ -4613,7 +4591,7 @@
       <c r="Q16" s="19">
         <v>6.4203448897037795E-4</v>
       </c>
-      <c r="S16" s="77"/>
+      <c r="S16" s="94"/>
       <c r="T16" s="45"/>
       <c r="U16" s="45"/>
       <c r="V16" s="16" t="s">
@@ -4633,7 +4611,7 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="89" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="40"/>
@@ -4653,7 +4631,7 @@
       <c r="H17" s="28">
         <v>1.4661160013996999E-2</v>
       </c>
-      <c r="J17" s="72" t="s">
+      <c r="J17" s="89" t="s">
         <v>15</v>
       </c>
       <c r="K17" s="40"/>
@@ -4673,7 +4651,7 @@
       <c r="Q17" s="27">
         <v>0.63226305707268105</v>
       </c>
-      <c r="S17" s="72" t="s">
+      <c r="S17" s="89" t="s">
         <v>21</v>
       </c>
       <c r="T17" s="40"/>
@@ -4695,7 +4673,7 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A18" s="73"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="3" t="s">
@@ -4713,7 +4691,7 @@
       <c r="H18" s="10">
         <v>1.03589205298071E-4</v>
       </c>
-      <c r="J18" s="73"/>
+      <c r="J18" s="90"/>
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="3" t="s">
@@ -4731,7 +4709,7 @@
       <c r="Q18" s="5">
         <v>0.63091798944421296</v>
       </c>
-      <c r="S18" s="73"/>
+      <c r="S18" s="90"/>
       <c r="T18" s="41"/>
       <c r="U18" s="41"/>
       <c r="V18" s="3" t="s">
@@ -4751,7 +4729,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" s="73"/>
+      <c r="A19" s="90"/>
       <c r="B19" s="41">
         <v>0.37</v>
       </c>
@@ -4773,7 +4751,7 @@
       <c r="H19" s="10">
         <v>3.4893820447861899E-2</v>
       </c>
-      <c r="J19" s="73"/>
+      <c r="J19" s="90"/>
       <c r="K19" s="41">
         <v>0.12</v>
       </c>
@@ -4795,7 +4773,7 @@
       <c r="Q19" s="5">
         <v>0.19006605256154599</v>
       </c>
-      <c r="S19" s="73"/>
+      <c r="S19" s="90"/>
       <c r="T19" s="41">
         <v>0.09</v>
       </c>
@@ -4819,7 +4797,7 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A20" s="73"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="3" t="s">
@@ -4837,7 +4815,7 @@
       <c r="H20" s="5">
         <v>0.58894272291956795</v>
       </c>
-      <c r="J20" s="73"/>
+      <c r="J20" s="90"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="3" t="s">
@@ -4855,7 +4833,7 @@
       <c r="Q20" s="5">
         <v>0.45770082770904802</v>
       </c>
-      <c r="S20" s="73"/>
+      <c r="S20" s="90"/>
       <c r="T20" s="41"/>
       <c r="U20" s="41"/>
       <c r="V20" s="3" t="s">
@@ -4875,7 +4853,7 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="74"/>
+      <c r="A21" s="91"/>
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="6" t="s">
@@ -4893,7 +4871,7 @@
       <c r="H21" s="8">
         <v>8.1306385386086505E-2</v>
       </c>
-      <c r="J21" s="74"/>
+      <c r="J21" s="91"/>
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
       <c r="M21" s="6" t="s">
@@ -4911,7 +4889,7 @@
       <c r="Q21" s="8">
         <v>0.17256483293313099</v>
       </c>
-      <c r="S21" s="74"/>
+      <c r="S21" s="91"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
       <c r="V21" s="6" t="s">
@@ -4931,7 +4909,7 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="92" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="43"/>
@@ -4951,7 +4929,7 @@
       <c r="H22" s="26">
         <v>0.156590362282719</v>
       </c>
-      <c r="J22" s="75" t="s">
+      <c r="J22" s="92" t="s">
         <v>16</v>
       </c>
       <c r="K22" s="43"/>
@@ -4971,7 +4949,7 @@
       <c r="Q22" s="26">
         <v>0.69885942821946401</v>
       </c>
-      <c r="S22" s="75" t="s">
+      <c r="S22" s="92" t="s">
         <v>22</v>
       </c>
       <c r="T22" s="43"/>
@@ -4993,7 +4971,7 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" s="76"/>
+      <c r="A23" s="93"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
       <c r="D23" s="13" t="s">
@@ -5011,7 +4989,7 @@
       <c r="H23" s="15">
         <v>0.904389521648304</v>
       </c>
-      <c r="J23" s="76"/>
+      <c r="J23" s="93"/>
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
       <c r="M23" s="13" t="s">
@@ -5029,7 +5007,7 @@
       <c r="Q23" s="15">
         <v>0.62584133799445296</v>
       </c>
-      <c r="S23" s="76"/>
+      <c r="S23" s="93"/>
       <c r="T23" s="44"/>
       <c r="U23" s="44"/>
       <c r="V23" s="13" t="s">
@@ -5049,7 +5027,7 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A24" s="76"/>
+      <c r="A24" s="93"/>
       <c r="B24" s="44">
         <v>0.1</v>
       </c>
@@ -5071,7 +5049,7 @@
       <c r="H24" s="15">
         <v>0.30569527576697603</v>
       </c>
-      <c r="J24" s="76"/>
+      <c r="J24" s="93"/>
       <c r="K24" s="44">
         <v>0.08</v>
       </c>
@@ -5093,7 +5071,7 @@
       <c r="Q24" s="15">
         <v>0.56359297147337195</v>
       </c>
-      <c r="S24" s="76"/>
+      <c r="S24" s="93"/>
       <c r="T24" s="44">
         <v>0.1</v>
       </c>
@@ -5117,7 +5095,7 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A25" s="76"/>
+      <c r="A25" s="93"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="13" t="s">
@@ -5135,7 +5113,7 @@
       <c r="H25" s="15">
         <v>0.68583510960772898</v>
       </c>
-      <c r="J25" s="76"/>
+      <c r="J25" s="93"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="13" t="s">
@@ -5153,7 +5131,7 @@
       <c r="Q25" s="15">
         <v>0.70588105337253604</v>
       </c>
-      <c r="S25" s="76"/>
+      <c r="S25" s="93"/>
       <c r="T25" s="44"/>
       <c r="U25" s="44"/>
       <c r="V25" s="13" t="s">
@@ -5173,7 +5151,7 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A26" s="77"/>
+      <c r="A26" s="94"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
       <c r="D26" s="16" t="s">
@@ -5191,7 +5169,7 @@
       <c r="H26" s="20">
         <v>0.41122866769062399</v>
       </c>
-      <c r="J26" s="77"/>
+      <c r="J26" s="94"/>
       <c r="K26" s="45"/>
       <c r="L26" s="45"/>
       <c r="M26" s="16" t="s">
@@ -5209,7 +5187,7 @@
       <c r="Q26" s="20">
         <v>0.24845922044221999</v>
       </c>
-      <c r="S26" s="77"/>
+      <c r="S26" s="94"/>
       <c r="T26" s="45"/>
       <c r="U26" s="45"/>
       <c r="V26" s="16" t="s">
@@ -5229,7 +5207,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="89" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="40"/>
@@ -5249,7 +5227,7 @@
       <c r="H27" s="28">
         <v>1.02956589885583E-2</v>
       </c>
-      <c r="J27" s="72" t="s">
+      <c r="J27" s="89" t="s">
         <v>17</v>
       </c>
       <c r="K27" s="40"/>
@@ -5269,7 +5247,7 @@
       <c r="Q27" s="27">
         <v>0.91086414946984995</v>
       </c>
-      <c r="S27" s="72" t="s">
+      <c r="S27" s="89" t="s">
         <v>23</v>
       </c>
       <c r="T27" s="40"/>
@@ -5291,7 +5269,7 @@
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A28" s="73"/>
+      <c r="A28" s="90"/>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
       <c r="D28" s="3" t="s">
@@ -5309,7 +5287,7 @@
       <c r="H28" s="10">
         <v>4.8954711894798199E-2</v>
       </c>
-      <c r="J28" s="73"/>
+      <c r="J28" s="90"/>
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="3" t="s">
@@ -5327,7 +5305,7 @@
       <c r="Q28" s="5">
         <v>0.95282317254778404</v>
       </c>
-      <c r="S28" s="73"/>
+      <c r="S28" s="90"/>
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="V28" s="3" t="s">
@@ -5347,7 +5325,7 @@
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A29" s="73"/>
+      <c r="A29" s="90"/>
       <c r="B29" s="41">
         <v>0.54</v>
       </c>
@@ -5369,7 +5347,7 @@
       <c r="H29" s="5">
         <v>0.60274047594928004</v>
       </c>
-      <c r="J29" s="73"/>
+      <c r="J29" s="90"/>
       <c r="K29" s="41">
         <v>0.68</v>
       </c>
@@ -5391,7 +5369,7 @@
       <c r="Q29" s="5">
         <v>0.72885199050288396</v>
       </c>
-      <c r="S29" s="73"/>
+      <c r="S29" s="90"/>
       <c r="T29" s="41">
         <v>0.05</v>
       </c>
@@ -5415,7 +5393,7 @@
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A30" s="73"/>
+      <c r="A30" s="90"/>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
       <c r="D30" s="3" t="s">
@@ -5433,7 +5411,7 @@
       <c r="H30" s="5">
         <v>0.100097196819914</v>
       </c>
-      <c r="J30" s="73"/>
+      <c r="J30" s="90"/>
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="3" t="s">
@@ -5451,7 +5429,7 @@
       <c r="Q30" s="5">
         <v>0.45481679394520702</v>
       </c>
-      <c r="S30" s="73"/>
+      <c r="S30" s="90"/>
       <c r="T30" s="41"/>
       <c r="U30" s="41"/>
       <c r="V30" s="3" t="s">
@@ -5471,7 +5449,7 @@
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A31" s="74"/>
+      <c r="A31" s="91"/>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
       <c r="D31" s="6" t="s">
@@ -5489,7 +5467,7 @@
       <c r="H31" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="74"/>
+      <c r="J31" s="91"/>
       <c r="K31" s="42"/>
       <c r="L31" s="42"/>
       <c r="M31" s="6" t="s">
@@ -5507,7 +5485,7 @@
       <c r="Q31" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="S31" s="74"/>
+      <c r="S31" s="91"/>
       <c r="T31" s="42"/>
       <c r="U31" s="42"/>
       <c r="V31" s="6" t="s">
@@ -5528,12 +5506,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
     <mergeCell ref="S27:S31"/>
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="J7:J11"/>
@@ -5546,6 +5518,12 @@
     <mergeCell ref="S12:S16"/>
     <mergeCell ref="S17:S21"/>
     <mergeCell ref="S22:S26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5896,13 +5874,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="78">
+      <c r="B2" s="95">
         <v>0.02</v>
       </c>
-      <c r="C2" s="78">
+      <c r="C2" s="95">
         <v>0.13</v>
       </c>
       <c r="D2" s="43" t="s">
@@ -5922,9 +5900,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="79"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
+      <c r="A3" s="96"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
       <c r="D3" s="45" t="s">
         <v>29</v>
       </c>
@@ -5942,13 +5920,13 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="84">
+      <c r="B4" s="97">
         <v>0.01</v>
       </c>
-      <c r="C4" s="84">
+      <c r="C4" s="97">
         <v>0.42</v>
       </c>
       <c r="D4" s="40" t="s">
@@ -5968,9 +5946,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="85"/>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="42" t="s">
         <v>29</v>
       </c>
@@ -5988,13 +5966,13 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="78">
+      <c r="B6" s="95">
         <v>0.08</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="95">
         <v>0.25</v>
       </c>
       <c r="D6" s="43" t="s">
@@ -6014,9 +5992,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="81"/>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+      <c r="A7" s="100"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
       <c r="D7" s="45" t="s">
         <v>29</v>
       </c>
@@ -6034,13 +6012,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="84">
+      <c r="B8" s="97">
         <v>0.03</v>
       </c>
-      <c r="C8" s="84">
+      <c r="C8" s="97">
         <v>0.15</v>
       </c>
       <c r="D8" s="40" t="s">
@@ -6060,9 +6038,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="42" t="s">
         <v>29</v>
       </c>
@@ -6080,13 +6058,13 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="78">
+      <c r="B10" s="95">
         <v>0.01</v>
       </c>
-      <c r="C10" s="78">
+      <c r="C10" s="95">
         <v>0.08</v>
       </c>
       <c r="D10" s="43" t="s">
@@ -6106,9 +6084,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="79"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="45" t="s">
         <v>29</v>
       </c>
@@ -6127,12 +6105,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
@@ -6142,6 +6114,12 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6152,66 +6130,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64F4DAD-9E02-44CC-9B21-7675E393CEAC}">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1:W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" style="86" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" style="86" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="86" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" style="86" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="86" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="86"/>
-    <col min="9" max="9" width="19" style="86" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.77734375" style="86" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="86" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.21875" style="86" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" style="86" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="86"/>
-    <col min="17" max="17" width="19" style="86" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.77734375" style="86" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.5546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" style="86" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.5546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.21875" style="86" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.88671875" style="86"/>
+    <col min="1" max="1" width="19" style="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="72" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" style="72" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="72" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="72"/>
+    <col min="9" max="9" width="19" style="72" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.77734375" style="72" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="72" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.21875" style="72" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="72" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="72"/>
+    <col min="17" max="17" width="19" style="72" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.77734375" style="72" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" style="72" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" style="72" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.21875" style="72" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.88671875" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="103" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="I1" s="99" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="I1" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="Q1" s="99" t="s">
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="Q1" s="103" t="s">
         <v>128</v>
       </c>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
     </row>
     <row r="2" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -6279,7 +6257,7 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="73" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="37">
@@ -6288,7 +6266,7 @@
       <c r="C3" s="37">
         <v>0.88131467557302301</v>
       </c>
-      <c r="D3" s="100">
+      <c r="D3" s="79">
         <v>-9.8019035084793801E-2</v>
       </c>
       <c r="E3" s="26">
@@ -6297,10 +6275,10 @@
       <c r="F3" s="37">
         <v>-6.3508284610398702</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="G3" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="93" t="s">
+      <c r="I3" s="73" t="s">
         <v>96</v>
       </c>
       <c r="J3" s="37">
@@ -6309,7 +6287,7 @@
       <c r="K3" s="37">
         <v>0.98269129564414703</v>
       </c>
-      <c r="L3" s="100">
+      <c r="L3" s="79">
         <v>-8.2719511879325094E-2</v>
       </c>
       <c r="M3" s="26">
@@ -6318,10 +6296,10 @@
       <c r="N3" s="37">
         <v>-6.8030361808973501</v>
       </c>
-      <c r="O3" s="101" t="s">
+      <c r="O3" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="93" t="s">
+      <c r="Q3" s="73" t="s">
         <v>91</v>
       </c>
       <c r="R3" s="37">
@@ -6344,137 +6322,137 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="87">
+      <c r="B4" s="14">
         <v>0.66710783984258804</v>
       </c>
-      <c r="C4" s="87">
+      <c r="C4" s="14">
         <v>0.69116857988539004</v>
       </c>
-      <c r="D4" s="88">
+      <c r="D4" s="22">
         <v>-8.1197517108981099E-2</v>
       </c>
-      <c r="E4" s="89">
+      <c r="E4" s="15">
         <v>1.7548183462441198E-2</v>
       </c>
-      <c r="F4" s="87">
+      <c r="F4" s="14">
         <v>-4.62711808790751</v>
       </c>
-      <c r="G4" s="107" t="s">
+      <c r="G4" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="94" t="s">
+      <c r="I4" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="87">
+      <c r="J4" s="14">
         <v>0.54095534054056704</v>
       </c>
-      <c r="K4" s="87">
+      <c r="K4" s="14">
         <v>0.54095534054056704</v>
       </c>
-      <c r="L4" s="88">
+      <c r="L4" s="22">
         <v>-6.2976256741974698E-2</v>
       </c>
-      <c r="M4" s="89">
+      <c r="M4" s="15">
         <v>1.8345248804811299E-2</v>
       </c>
-      <c r="N4" s="87">
+      <c r="N4" s="14">
         <v>-3.4328374290273</v>
       </c>
-      <c r="O4" s="102" t="s">
+      <c r="O4" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="94" t="s">
+      <c r="Q4" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="R4" s="87">
+      <c r="R4" s="14">
         <v>0.34637488087420998</v>
       </c>
-      <c r="S4" s="87">
+      <c r="S4" s="14">
         <v>0.34637488087420998</v>
       </c>
-      <c r="T4" s="88">
+      <c r="T4" s="22">
         <v>-6.2798594397034002E-2</v>
       </c>
-      <c r="U4" s="89">
+      <c r="U4" s="15">
         <v>2.6010263558101199E-2</v>
       </c>
-      <c r="V4" s="87">
+      <c r="V4" s="14">
         <v>-2.4143774728293601</v>
       </c>
-      <c r="W4" s="88">
+      <c r="W4" s="22">
         <v>1.57621233813394E-2</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="87">
+      <c r="B5" s="14">
         <v>0.43722158845070103</v>
       </c>
-      <c r="C5" s="87">
+      <c r="C5" s="14">
         <v>0.68276650095009295</v>
       </c>
-      <c r="D5" s="88">
+      <c r="D5" s="22">
         <v>-6.9447617835114106E-2</v>
       </c>
-      <c r="E5" s="89">
+      <c r="E5" s="15">
         <v>1.78360931831071E-2</v>
       </c>
-      <c r="F5" s="87">
+      <c r="F5" s="14">
         <v>-3.8936563698203401</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="G5" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="94" t="s">
+      <c r="I5" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="87">
+      <c r="J5" s="14">
         <v>0.41544290529841699</v>
       </c>
-      <c r="K5" s="87">
+      <c r="K5" s="14">
         <v>0.88424319415291397</v>
       </c>
-      <c r="L5" s="88">
+      <c r="L5" s="22">
         <v>-9.7935331414033197E-2</v>
       </c>
-      <c r="M5" s="89">
+      <c r="M5" s="15">
         <v>1.55869322829492E-2</v>
       </c>
-      <c r="N5" s="87">
+      <c r="N5" s="14">
         <v>-6.2831691083412498</v>
       </c>
-      <c r="O5" s="102" t="s">
+      <c r="O5" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="94" t="s">
+      <c r="Q5" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="R5" s="87">
+      <c r="R5" s="14">
         <v>3.1638961137750998E-2</v>
       </c>
-      <c r="S5" s="87">
+      <c r="S5" s="14">
         <v>0.732389756378788</v>
       </c>
-      <c r="T5" s="89">
+      <c r="T5" s="15">
         <v>3.6323373499386698E-2</v>
       </c>
-      <c r="U5" s="89">
+      <c r="U5" s="15">
         <v>3.18515149172156E-2</v>
       </c>
-      <c r="V5" s="87">
+      <c r="V5" s="14">
         <v>1.14039704528321</v>
       </c>
-      <c r="W5" s="89">
+      <c r="W5" s="15">
         <v>0.25412092330939401</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="75" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="18">
@@ -6492,54 +6470,54 @@
       <c r="F6" s="18">
         <v>-18.514678615668</v>
       </c>
-      <c r="G6" s="108" t="s">
+      <c r="G6" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="94" t="s">
+      <c r="I6" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="87">
+      <c r="J6" s="14">
         <v>1.9533976684702001E-2</v>
       </c>
-      <c r="K6" s="87">
+      <c r="K6" s="14">
         <v>0.27512693440407698</v>
       </c>
-      <c r="L6" s="89">
+      <c r="L6" s="15">
         <v>-1.34765218865127E-2</v>
       </c>
-      <c r="M6" s="89">
+      <c r="M6" s="15">
         <v>3.1028762113403201E-2</v>
       </c>
-      <c r="N6" s="87">
+      <c r="N6" s="14">
         <v>-0.43432354269432299</v>
       </c>
-      <c r="O6" s="89">
+      <c r="O6" s="15">
         <v>0.66405351013498803</v>
       </c>
-      <c r="Q6" s="94" t="s">
+      <c r="Q6" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="R6" s="87">
+      <c r="R6" s="14">
         <v>1.0107195353671601E-3</v>
       </c>
-      <c r="S6" s="87">
+      <c r="S6" s="14">
         <v>0.76172606542772003</v>
       </c>
-      <c r="T6" s="89">
+      <c r="T6" s="15">
         <v>-4.9904882640520697E-3</v>
       </c>
-      <c r="U6" s="89">
+      <c r="U6" s="15">
         <v>2.3103066821470002E-2</v>
       </c>
-      <c r="V6" s="87">
+      <c r="V6" s="14">
         <v>-0.21600977491933401</v>
       </c>
-      <c r="W6" s="89">
+      <c r="W6" s="15">
         <v>0.82898012815102995</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="76" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="38">
@@ -6557,10 +6535,10 @@
       <c r="F7" s="38">
         <v>-4.3548347001684196</v>
       </c>
-      <c r="G7" s="109" t="s">
+      <c r="G7" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="75" t="s">
         <v>100</v>
       </c>
       <c r="J7" s="18">
@@ -6581,7 +6559,7 @@
       <c r="O7" s="19">
         <v>5.5973949370031802E-3</v>
       </c>
-      <c r="Q7" s="95" t="s">
+      <c r="Q7" s="75" t="s">
         <v>95</v>
       </c>
       <c r="R7" s="18">
@@ -6604,28 +6582,28 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="90">
+      <c r="B8" s="4">
         <v>0.37442313318574599</v>
       </c>
-      <c r="C8" s="90">
+      <c r="C8" s="4">
         <v>0.69846202856958906</v>
       </c>
-      <c r="D8" s="91">
+      <c r="D8" s="10">
         <v>-4.7330607553170798E-2</v>
       </c>
-      <c r="E8" s="92">
+      <c r="E8" s="5">
         <v>1.36650135243821E-2</v>
       </c>
-      <c r="F8" s="90">
+      <c r="F8" s="4">
         <v>-3.4636341536523299</v>
       </c>
-      <c r="G8" s="110" t="s">
+      <c r="G8" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="96" t="s">
+      <c r="I8" s="76" t="s">
         <v>101</v>
       </c>
       <c r="J8" s="38">
@@ -6646,7 +6624,7 @@
       <c r="O8" s="27">
         <v>0.31407250314297303</v>
       </c>
-      <c r="Q8" s="96" t="s">
+      <c r="Q8" s="76" t="s">
         <v>96</v>
       </c>
       <c r="R8" s="38">
@@ -6669,72 +6647,72 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="90">
+      <c r="B9" s="4">
         <v>0.33918961529897002</v>
       </c>
-      <c r="C9" s="90">
+      <c r="C9" s="4">
         <v>0.75550333014474902</v>
       </c>
-      <c r="D9" s="91">
+      <c r="D9" s="10">
         <v>-8.4221681329308906E-2</v>
       </c>
-      <c r="E9" s="92">
+      <c r="E9" s="5">
         <v>2.1559702556969099E-2</v>
       </c>
-      <c r="F9" s="90">
+      <c r="F9" s="4">
         <v>-3.9064398549452299</v>
       </c>
-      <c r="G9" s="110" t="s">
+      <c r="G9" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="97" t="s">
+      <c r="I9" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="J9" s="90">
+      <c r="J9" s="4">
         <v>0.101603224848101</v>
       </c>
-      <c r="K9" s="90">
+      <c r="K9" s="4">
         <v>0.101603224848101</v>
       </c>
-      <c r="L9" s="92">
+      <c r="L9" s="5">
         <v>-3.5420093581485901E-2</v>
       </c>
-      <c r="M9" s="92">
+      <c r="M9" s="5">
         <v>3.3306580737482598E-2</v>
       </c>
-      <c r="N9" s="90">
+      <c r="N9" s="4">
         <v>-1.0634563139537401</v>
       </c>
-      <c r="O9" s="92">
+      <c r="O9" s="5">
         <v>0.28757506642501701</v>
       </c>
-      <c r="Q9" s="97" t="s">
+      <c r="Q9" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="R9" s="90">
+      <c r="R9" s="4">
         <v>0.354908032017622</v>
       </c>
-      <c r="S9" s="90">
+      <c r="S9" s="4">
         <v>0.354908032017622</v>
       </c>
-      <c r="T9" s="91">
+      <c r="T9" s="10">
         <v>-5.4365749028637299E-2</v>
       </c>
-      <c r="U9" s="92">
+      <c r="U9" s="5">
         <v>2.2099473980815999E-2</v>
       </c>
-      <c r="V9" s="90">
+      <c r="V9" s="4">
         <v>-2.4600471973147799</v>
       </c>
-      <c r="W9" s="91">
+      <c r="W9" s="10">
         <v>1.38918745547432E-2</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="78" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="7">
@@ -6755,137 +6733,137 @@
       <c r="G10" s="12">
         <v>2.7756055244445601E-2</v>
       </c>
-      <c r="I10" s="97" t="s">
+      <c r="I10" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="J10" s="90">
+      <c r="J10" s="4">
         <v>0.15756520680198799</v>
       </c>
-      <c r="K10" s="90">
+      <c r="K10" s="4">
         <v>0.73108462704673005</v>
       </c>
-      <c r="L10" s="91">
+      <c r="L10" s="10">
         <v>-5.0350828191650501E-2</v>
       </c>
-      <c r="M10" s="92">
+      <c r="M10" s="5">
         <v>1.98329779456787E-2</v>
       </c>
-      <c r="N10" s="90">
+      <c r="N10" s="4">
         <v>-2.53874271072949</v>
       </c>
-      <c r="O10" s="91">
+      <c r="O10" s="10">
         <v>1.1125160556327601E-2</v>
       </c>
-      <c r="Q10" s="97" t="s">
+      <c r="Q10" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="R10" s="90">
+      <c r="R10" s="4">
         <v>1.7616663646243699E-2</v>
       </c>
-      <c r="S10" s="90">
+      <c r="S10" s="4">
         <v>0.82252804997691598</v>
       </c>
-      <c r="T10" s="92">
+      <c r="T10" s="5">
         <v>2.5971980464054901E-2</v>
       </c>
-      <c r="U10" s="92">
+      <c r="U10" s="5">
         <v>2.4854884787504101E-2</v>
       </c>
-      <c r="V10" s="90">
+      <c r="V10" s="4">
         <v>1.0449447135282</v>
       </c>
-      <c r="W10" s="92">
+      <c r="W10" s="5">
         <v>0.29604852248576302</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="87">
+      <c r="B11" s="14">
         <v>0.26646274201391701</v>
       </c>
-      <c r="C11" s="87">
+      <c r="C11" s="14">
         <v>0.83462650200239996</v>
       </c>
-      <c r="D11" s="88">
+      <c r="D11" s="22">
         <v>-9.2511900443405501E-2</v>
       </c>
-      <c r="E11" s="89">
+      <c r="E11" s="15">
         <v>2.1974346587643401E-2</v>
       </c>
-      <c r="F11" s="87">
+      <c r="F11" s="14">
         <v>-4.2099955088278698</v>
       </c>
-      <c r="G11" s="107" t="s">
+      <c r="G11" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="97" t="s">
+      <c r="I11" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="90">
+      <c r="J11" s="4">
         <v>0.18328422474660599</v>
       </c>
-      <c r="K11" s="90">
+      <c r="K11" s="4">
         <v>0.63382211688654899</v>
       </c>
-      <c r="L11" s="92">
+      <c r="L11" s="5">
         <v>-5.5787618156151297E-2</v>
       </c>
-      <c r="M11" s="92">
+      <c r="M11" s="5">
         <v>2.9803846025700399E-2</v>
       </c>
-      <c r="N11" s="90">
+      <c r="N11" s="4">
         <v>-1.87182614311068</v>
       </c>
-      <c r="O11" s="92">
+      <c r="O11" s="5">
         <v>6.1230660171244698E-2</v>
       </c>
-      <c r="Q11" s="97" t="s">
+      <c r="Q11" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="R11" s="90">
+      <c r="R11" s="4">
         <v>4.7238136378487203E-3</v>
       </c>
-      <c r="S11" s="90">
+      <c r="S11" s="4">
         <v>0.75013495507449501</v>
       </c>
-      <c r="T11" s="92">
+      <c r="T11" s="5">
         <v>-8.9291439480759204E-3</v>
       </c>
-      <c r="U11" s="92">
+      <c r="U11" s="5">
         <v>1.9580323199494501E-2</v>
       </c>
-      <c r="V11" s="90">
+      <c r="V11" s="4">
         <v>-0.45602638205208101</v>
       </c>
-      <c r="W11" s="92">
+      <c r="W11" s="5">
         <v>0.64837100708135498</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="87">
+      <c r="B12" s="14">
         <v>8.4171884694533294E-2</v>
       </c>
-      <c r="C12" s="87">
+      <c r="C12" s="14">
         <v>0.235545162308925</v>
       </c>
-      <c r="D12" s="89">
+      <c r="D12" s="15">
         <v>-2.83530127645054E-2</v>
       </c>
-      <c r="E12" s="89">
+      <c r="E12" s="15">
         <v>2.7254372250901101E-2</v>
       </c>
-      <c r="F12" s="87">
+      <c r="F12" s="14">
         <v>-1.0403106152469901</v>
       </c>
-      <c r="G12" s="89">
+      <c r="G12" s="15">
         <v>0.298195613987704</v>
       </c>
-      <c r="I12" s="98" t="s">
+      <c r="I12" s="78" t="s">
         <v>105</v>
       </c>
       <c r="J12" s="7">
@@ -6906,7 +6884,7 @@
       <c r="O12" s="8">
         <v>0.10399222281932501</v>
       </c>
-      <c r="Q12" s="98" t="s">
+      <c r="Q12" s="78" t="s">
         <v>100</v>
       </c>
       <c r="R12" s="7">
@@ -6929,72 +6907,72 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="87">
+      <c r="B13" s="14">
         <v>0.26412414648485699</v>
       </c>
-      <c r="C13" s="87">
+      <c r="C13" s="14">
         <v>0.77495461837118496</v>
       </c>
-      <c r="D13" s="88">
+      <c r="D13" s="22">
         <v>-7.0813458301321006E-2</v>
       </c>
-      <c r="E13" s="89">
+      <c r="E13" s="15">
         <v>1.9708358833297999E-2</v>
       </c>
-      <c r="F13" s="87">
+      <c r="F13" s="14">
         <v>-3.59306723103089</v>
       </c>
-      <c r="G13" s="107" t="s">
+      <c r="G13" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="94" t="s">
+      <c r="I13" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="J13" s="87">
+      <c r="J13" s="14">
         <v>0.38932878875545501</v>
       </c>
-      <c r="K13" s="87">
+      <c r="K13" s="14">
         <v>0.57064987846292703</v>
       </c>
-      <c r="L13" s="89">
+      <c r="L13" s="15">
         <v>-0.18126241235592999</v>
       </c>
-      <c r="M13" s="89">
+      <c r="M13" s="15">
         <v>9.3535906220054005E-2</v>
       </c>
-      <c r="N13" s="87">
+      <c r="N13" s="14">
         <v>-1.9378912300212201</v>
       </c>
-      <c r="O13" s="89">
+      <c r="O13" s="15">
         <v>5.2636494155608997E-2</v>
       </c>
-      <c r="Q13" s="94" t="s">
+      <c r="Q13" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="R13" s="87">
-        <v>9.9575877666512796E-2</v>
-      </c>
-      <c r="S13" s="87">
-        <v>9.9575877666512796E-2</v>
-      </c>
-      <c r="T13" s="89">
-        <v>-7.2883661044314402E-2</v>
-      </c>
-      <c r="U13" s="89">
-        <v>6.60815659856369E-2</v>
-      </c>
-      <c r="V13" s="87">
-        <v>-1.10293483450674</v>
-      </c>
-      <c r="W13" s="89">
-        <v>0.27005546538923098</v>
+      <c r="R13" s="14">
+        <v>4.5165638283528098E-2</v>
+      </c>
+      <c r="S13" s="14">
+        <v>0.401445866536773</v>
+      </c>
+      <c r="T13" s="15">
+        <v>5.6646123525934199E-2</v>
+      </c>
+      <c r="U13" s="15">
+        <v>6.2175815984151402E-2</v>
+      </c>
+      <c r="V13" s="14">
+        <v>0.91106361258488699</v>
+      </c>
+      <c r="W13" s="15">
+        <v>0.36226185741713901</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="75" t="s">
         <v>110</v>
       </c>
       <c r="B14" s="18">
@@ -7015,51 +6993,51 @@
       <c r="G14" s="19">
         <v>7.76072663314942E-3</v>
       </c>
-      <c r="I14" s="94" t="s">
+      <c r="I14" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="J14" s="87">
+      <c r="J14" s="14">
         <v>9.8207379389655694E-2</v>
       </c>
-      <c r="K14" s="87">
+      <c r="K14" s="14">
         <v>0.24063340614060799</v>
       </c>
-      <c r="L14" s="89">
+      <c r="L14" s="15">
         <v>-4.8336095435263501E-2</v>
       </c>
-      <c r="M14" s="89">
+      <c r="M14" s="15">
         <v>4.2859419212394598E-2</v>
       </c>
-      <c r="N14" s="87">
+      <c r="N14" s="14">
         <v>-1.1277823247144001</v>
       </c>
-      <c r="O14" s="89">
+      <c r="O14" s="15">
         <v>0.259411859844703</v>
       </c>
-      <c r="Q14" s="94" t="s">
+      <c r="Q14" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="R14" s="87">
-        <v>9.1057801525080695E-2</v>
-      </c>
-      <c r="S14" s="87">
-        <v>0.41774973683205502</v>
-      </c>
-      <c r="T14" s="89">
-        <v>7.7508190238214494E-2</v>
-      </c>
-      <c r="U14" s="89">
-        <v>5.9094562317178398E-2</v>
-      </c>
-      <c r="V14" s="87">
-        <v>1.31159597768412</v>
-      </c>
-      <c r="W14" s="89">
-        <v>0.18965649091679801</v>
+      <c r="R14" s="14">
+        <v>3.22213452033831E-2</v>
+      </c>
+      <c r="S14" s="14">
+        <v>3.22213452033831E-2</v>
+      </c>
+      <c r="T14" s="15">
+        <v>4.3292058558877501E-2</v>
+      </c>
+      <c r="U14" s="15">
+        <v>7.1536564623769394E-2</v>
+      </c>
+      <c r="V14" s="14">
+        <v>0.60517385460935103</v>
+      </c>
+      <c r="W14" s="15">
+        <v>0.54506348602683696</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="76" t="s">
         <v>111</v>
       </c>
       <c r="B15" s="38">
@@ -7080,137 +7058,137 @@
       <c r="G15" s="28">
         <v>2.97548504107359E-2</v>
       </c>
-      <c r="I15" s="94" t="s">
+      <c r="I15" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="J15" s="87">
+      <c r="J15" s="14">
         <v>8.7920706129776094E-2</v>
       </c>
-      <c r="K15" s="87">
+      <c r="K15" s="14">
         <v>0.58608089905612204</v>
       </c>
-      <c r="L15" s="89">
+      <c r="L15" s="15">
         <v>-5.84422134248474E-2</v>
       </c>
-      <c r="M15" s="89">
+      <c r="M15" s="15">
         <v>3.8233359786043898E-2</v>
       </c>
-      <c r="N15" s="87">
+      <c r="N15" s="14">
         <v>-1.52856598927987</v>
       </c>
-      <c r="O15" s="89">
+      <c r="O15" s="15">
         <v>0.12637207281625701</v>
       </c>
-      <c r="Q15" s="94" t="s">
+      <c r="Q15" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="R15" s="87">
-        <v>7.3859723705051297E-2</v>
-      </c>
-      <c r="S15" s="87">
-        <v>0.163151144842691</v>
-      </c>
-      <c r="T15" s="89">
-        <v>5.1694166598557897E-2</v>
-      </c>
-      <c r="U15" s="89">
-        <v>5.2464419191421897E-2</v>
-      </c>
-      <c r="V15" s="87">
-        <v>0.98531857200108197</v>
-      </c>
-      <c r="W15" s="89">
-        <v>0.32446761294080001</v>
+      <c r="R15" s="14">
+        <v>0.10291303606636799</v>
+      </c>
+      <c r="S15" s="14">
+        <v>0.10291303606636799</v>
+      </c>
+      <c r="T15" s="15">
+        <v>0.105484182223472</v>
+      </c>
+      <c r="U15" s="15">
+        <v>9.3901617939857004E-2</v>
+      </c>
+      <c r="V15" s="14">
+        <v>1.12334786703072</v>
+      </c>
+      <c r="W15" s="15">
+        <v>0.26128978175907203</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="90">
+      <c r="B16" s="4">
         <v>0.25628763704936902</v>
       </c>
-      <c r="C16" s="90">
+      <c r="C16" s="4">
         <v>0.25628763704936902</v>
       </c>
-      <c r="D16" s="92">
+      <c r="D16" s="5">
         <v>6.6542971557223801E-2</v>
       </c>
-      <c r="E16" s="92">
+      <c r="E16" s="5">
         <v>3.5846013409580997E-2</v>
       </c>
-      <c r="F16" s="90">
+      <c r="F16" s="4">
         <v>1.8563562646952001</v>
       </c>
-      <c r="G16" s="92">
+      <c r="G16" s="5">
         <v>6.3402794230564205E-2</v>
       </c>
-      <c r="I16" s="94" t="s">
+      <c r="I16" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="J16" s="87">
+      <c r="J16" s="14">
         <v>0.22467498765110999</v>
       </c>
-      <c r="K16" s="87">
+      <c r="K16" s="14">
         <v>0.23449139622892201</v>
       </c>
-      <c r="L16" s="89">
+      <c r="L16" s="15">
         <v>-4.9190359922241703E-2</v>
       </c>
-      <c r="M16" s="89">
+      <c r="M16" s="15">
         <v>3.4318528271432398E-2</v>
       </c>
-      <c r="N16" s="87">
+      <c r="N16" s="14">
         <v>-1.43334701107183</v>
       </c>
-      <c r="O16" s="89">
+      <c r="O16" s="15">
         <v>0.15175869343675799</v>
       </c>
-      <c r="Q16" s="94" t="s">
+      <c r="Q16" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="R16" s="87">
-        <v>6.83307397796886E-4</v>
-      </c>
-      <c r="S16" s="87">
-        <v>0.33652331172221001</v>
-      </c>
-      <c r="T16" s="89">
-        <v>-5.2837806432061299E-3</v>
-      </c>
-      <c r="U16" s="89">
-        <v>4.9642450308114497E-2</v>
-      </c>
-      <c r="V16" s="87">
-        <v>-0.106436741345591</v>
-      </c>
-      <c r="W16" s="89">
-        <v>0.91523584325324603</v>
+      <c r="R16" s="14">
+        <v>0.13893617771941599</v>
+      </c>
+      <c r="S16" s="14">
+        <v>0.13893617771941599</v>
+      </c>
+      <c r="T16" s="15">
+        <v>0.122744776446175</v>
+      </c>
+      <c r="U16" s="15">
+        <v>9.21333101305358E-2</v>
+      </c>
+      <c r="V16" s="14">
+        <v>1.3322518888366099</v>
+      </c>
+      <c r="W16" s="15">
+        <v>0.18277743084204801</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="90">
+      <c r="B17" s="4">
         <v>6.5515203743213096E-2</v>
       </c>
-      <c r="C17" s="90">
+      <c r="C17" s="4">
         <v>6.5515203743213096E-2</v>
       </c>
-      <c r="D17" s="92">
+      <c r="D17" s="5">
         <v>2.1089191579322299E-2</v>
       </c>
-      <c r="E17" s="92">
+      <c r="E17" s="5">
         <v>2.4014782713818499E-2</v>
       </c>
-      <c r="F17" s="90">
+      <c r="F17" s="4">
         <v>0.87817540681670303</v>
       </c>
-      <c r="G17" s="92">
+      <c r="G17" s="5">
         <v>0.37984853607715602</v>
       </c>
-      <c r="I17" s="95" t="s">
+      <c r="I17" s="75" t="s">
         <v>110</v>
       </c>
       <c r="J17" s="18">
@@ -7231,30 +7209,30 @@
       <c r="O17" s="20">
         <v>0.16984067724777799</v>
       </c>
-      <c r="Q17" s="95" t="s">
+      <c r="Q17" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="R17" s="18">
-        <v>7.8784432890102903E-3</v>
-      </c>
-      <c r="S17" s="18">
-        <v>0.178996798205524</v>
-      </c>
-      <c r="T17" s="20">
-        <v>-1.99248073927208E-2</v>
-      </c>
-      <c r="U17" s="20">
-        <v>6.1326758214875897E-2</v>
-      </c>
-      <c r="V17" s="18">
-        <v>-0.324895819911246</v>
-      </c>
-      <c r="W17" s="20">
-        <v>0.74525992065149105</v>
+      <c r="R17" s="14">
+        <v>3.5473197707425803E-2</v>
+      </c>
+      <c r="S17" s="14">
+        <v>7.2853369014679994E-2</v>
+      </c>
+      <c r="T17" s="15">
+        <v>6.4594188471490094E-2</v>
+      </c>
+      <c r="U17" s="15">
+        <v>9.9568312415508495E-2</v>
+      </c>
+      <c r="V17" s="14">
+        <v>0.648742425219904</v>
+      </c>
+      <c r="W17" s="15">
+        <v>0.51650487728265904</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="78" t="s">
         <v>115</v>
       </c>
       <c r="B18" s="7">
@@ -7275,7 +7253,7 @@
       <c r="G18" s="8">
         <v>0.53909864335053403</v>
       </c>
-      <c r="I18" s="96" t="s">
+      <c r="I18" s="76" t="s">
         <v>111</v>
       </c>
       <c r="J18" s="38">
@@ -7296,7 +7274,7 @@
       <c r="O18" s="28">
         <v>1.91185992134018E-2</v>
       </c>
-      <c r="Q18" s="96" t="s">
+      <c r="Q18" s="76" t="s">
         <v>106</v>
       </c>
       <c r="R18" s="38">
@@ -7319,202 +7297,202 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="94" t="s">
+      <c r="A19" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="87">
+      <c r="B19" s="14">
         <v>9.5581582708037793E-2</v>
       </c>
-      <c r="C19" s="87">
+      <c r="C19" s="14">
         <v>0.34026101597870301</v>
       </c>
-      <c r="D19" s="89">
+      <c r="D19" s="15">
         <v>-5.6115551636423799E-3</v>
       </c>
-      <c r="E19" s="89">
+      <c r="E19" s="15">
         <v>4.4451442494566002E-3</v>
       </c>
-      <c r="F19" s="87">
+      <c r="F19" s="14">
         <v>-1.26240113902454</v>
       </c>
-      <c r="G19" s="89">
+      <c r="G19" s="15">
         <v>0.206804479579376</v>
       </c>
-      <c r="I19" s="97" t="s">
+      <c r="I19" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="J19" s="90">
+      <c r="J19" s="4">
         <v>2.4922759350102699E-2</v>
       </c>
-      <c r="K19" s="90">
+      <c r="K19" s="4">
         <v>0.60104715813802001</v>
       </c>
-      <c r="L19" s="92">
+      <c r="L19" s="5">
         <v>-2.93652208942441E-2</v>
       </c>
-      <c r="M19" s="92">
+      <c r="M19" s="5">
         <v>3.7838301756401203E-2</v>
       </c>
-      <c r="N19" s="90">
+      <c r="N19" s="4">
         <v>-0.77607132273784696</v>
       </c>
-      <c r="O19" s="92">
+      <c r="O19" s="5">
         <v>0.43770687490134502</v>
       </c>
-      <c r="Q19" s="97" t="s">
+      <c r="Q19" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="R19" s="90">
+      <c r="R19" s="4">
         <v>8.5901561933159705E-4</v>
       </c>
-      <c r="S19" s="90">
+      <c r="S19" s="4">
         <v>6.95694665450486E-2</v>
       </c>
-      <c r="T19" s="92">
+      <c r="T19" s="5">
         <v>4.5633440472272104E-3</v>
       </c>
-      <c r="U19" s="92">
+      <c r="U19" s="5">
         <v>4.5282283268598698E-2</v>
       </c>
-      <c r="V19" s="90">
+      <c r="V19" s="4">
         <v>0.100775484755463</v>
       </c>
-      <c r="W19" s="92">
+      <c r="W19" s="5">
         <v>0.91972868808040498</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="94" t="s">
+      <c r="A20" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="87">
+      <c r="B20" s="14">
         <v>0.28075361111592501</v>
       </c>
-      <c r="C20" s="87">
+      <c r="C20" s="14">
         <v>0.28075361111592501</v>
       </c>
-      <c r="D20" s="88">
+      <c r="D20" s="22">
         <v>2.90715235400031E-2</v>
       </c>
-      <c r="E20" s="89">
+      <c r="E20" s="15">
         <v>1.47144475693076E-2</v>
       </c>
-      <c r="F20" s="87">
+      <c r="F20" s="14">
         <v>1.97571287695791</v>
       </c>
-      <c r="G20" s="88">
+      <c r="G20" s="22">
         <v>4.8187305655134502E-2</v>
       </c>
-      <c r="I20" s="97" t="s">
+      <c r="I20" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="J20" s="90">
+      <c r="J20" s="4">
         <v>3.7945554577965101E-3</v>
       </c>
-      <c r="K20" s="90">
+      <c r="K20" s="4">
         <v>0.79815728626245397</v>
       </c>
-      <c r="L20" s="92">
+      <c r="L20" s="5">
         <v>-1.3825086280082E-2</v>
       </c>
-      <c r="M20" s="92">
+      <c r="M20" s="5">
         <v>3.0401680726775699E-2</v>
       </c>
-      <c r="N20" s="90">
+      <c r="N20" s="4">
         <v>-0.45474743335179502</v>
       </c>
-      <c r="O20" s="92">
+      <c r="O20" s="5">
         <v>0.64929095188022901</v>
       </c>
-      <c r="Q20" s="97" t="s">
+      <c r="Q20" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="R20" s="90">
+      <c r="R20" s="4">
         <v>0.13708332140079299</v>
       </c>
-      <c r="S20" s="90">
+      <c r="S20" s="4">
         <v>0.13708332140079299</v>
       </c>
-      <c r="T20" s="92">
+      <c r="T20" s="5">
         <v>5.3209105457176498E-2</v>
       </c>
-      <c r="U20" s="92">
+      <c r="U20" s="5">
         <v>4.0251469248442397E-2</v>
       </c>
-      <c r="V20" s="90">
+      <c r="V20" s="4">
         <v>1.3219170989450399</v>
       </c>
-      <c r="W20" s="92">
+      <c r="W20" s="5">
         <v>0.18619575791306101</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="87">
+      <c r="B21" s="14">
         <v>0.100227862438392</v>
       </c>
-      <c r="C21" s="87">
+      <c r="C21" s="14">
         <v>0.34512518070174403</v>
       </c>
-      <c r="D21" s="89">
+      <c r="D21" s="15">
         <v>-4.1669195485705803E-3</v>
       </c>
-      <c r="E21" s="89">
+      <c r="E21" s="15">
         <v>3.2114686338049702E-3</v>
       </c>
-      <c r="F21" s="87">
+      <c r="F21" s="14">
         <v>-1.2975121427960401</v>
       </c>
-      <c r="G21" s="89">
+      <c r="G21" s="15">
         <v>0.194455029826578</v>
       </c>
-      <c r="I21" s="97" t="s">
+      <c r="I21" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="J21" s="90">
+      <c r="J21" s="4">
         <v>9.2963834519367797E-3</v>
       </c>
-      <c r="K21" s="90">
+      <c r="K21" s="4">
         <v>0.79204737965475003</v>
       </c>
-      <c r="L21" s="92">
+      <c r="L21" s="5">
         <v>-1.24332971375217E-2</v>
       </c>
-      <c r="M21" s="92">
+      <c r="M21" s="5">
         <v>2.2226059716351099E-2</v>
       </c>
-      <c r="N21" s="90">
+      <c r="N21" s="4">
         <v>-0.55940176964317401</v>
       </c>
-      <c r="O21" s="92">
+      <c r="O21" s="5">
         <v>0.57588755391885205</v>
       </c>
-      <c r="Q21" s="97" t="s">
+      <c r="Q21" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="R21" s="90">
+      <c r="R21" s="4">
         <v>4.1082040598559001E-2</v>
       </c>
-      <c r="S21" s="90">
+      <c r="S21" s="4">
         <v>0.31416602684086697</v>
       </c>
-      <c r="T21" s="92">
+      <c r="T21" s="5">
         <v>3.0220272736632699E-2</v>
       </c>
-      <c r="U21" s="92">
+      <c r="U21" s="5">
         <v>3.7229356565358002E-2</v>
       </c>
-      <c r="V21" s="90">
+      <c r="V21" s="4">
         <v>0.81173234040667597</v>
       </c>
-      <c r="W21" s="92">
+      <c r="W21" s="5">
         <v>0.416945232950235</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="75" t="s">
         <v>120</v>
       </c>
       <c r="B22" s="18">
@@ -7535,7 +7513,7 @@
       <c r="G22" s="20">
         <v>0.80710619957312102</v>
       </c>
-      <c r="I22" s="98" t="s">
+      <c r="I22" s="78" t="s">
         <v>115</v>
       </c>
       <c r="J22" s="7">
@@ -7556,7 +7534,7 @@
       <c r="O22" s="8">
         <v>0.97483878997533202</v>
       </c>
-      <c r="Q22" s="98" t="s">
+      <c r="Q22" s="78" t="s">
         <v>110</v>
       </c>
       <c r="R22" s="7">
@@ -7579,7 +7557,7 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="76" t="s">
         <v>121</v>
       </c>
       <c r="B23" s="38">
@@ -7600,181 +7578,181 @@
       <c r="G23" s="28">
         <v>5.5683932015979697E-3</v>
       </c>
-      <c r="I23" s="94" t="s">
+      <c r="I23" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="87">
+      <c r="J23" s="14">
         <v>0.52338442286440101</v>
       </c>
-      <c r="K23" s="87">
+      <c r="K23" s="14">
         <v>0.52338442286440101</v>
       </c>
-      <c r="L23" s="88">
+      <c r="L23" s="22">
         <v>-0.14919890369591601</v>
       </c>
-      <c r="M23" s="89">
+      <c r="M23" s="15">
         <v>6.3672858815922107E-2</v>
       </c>
-      <c r="N23" s="87">
+      <c r="N23" s="14">
         <v>-2.3432103799084798</v>
       </c>
-      <c r="O23" s="88">
+      <c r="O23" s="22">
         <v>1.91185992134018E-2</v>
       </c>
-      <c r="Q23" s="94" t="s">
+      <c r="Q23" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="R23" s="87">
+      <c r="R23" s="14">
         <v>1.1420688224372699E-2</v>
       </c>
-      <c r="S23" s="87">
+      <c r="S23" s="14">
         <v>0.44006375730484798</v>
       </c>
-      <c r="T23" s="89">
+      <c r="T23" s="15">
         <v>1.3465919201208499E-2</v>
       </c>
-      <c r="U23" s="89">
+      <c r="U23" s="15">
         <v>2.8429080494077601E-2</v>
       </c>
-      <c r="V23" s="87">
+      <c r="V23" s="14">
         <v>0.47366706791708302</v>
       </c>
-      <c r="W23" s="89">
+      <c r="W23" s="15">
         <v>0.63573734083545197</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="97" t="s">
+      <c r="A24" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="B24" s="90">
+      <c r="B24" s="4">
         <v>0.61318316824936403</v>
       </c>
-      <c r="C24" s="90">
+      <c r="C24" s="4">
         <v>0.61318316824936403</v>
       </c>
-      <c r="D24" s="91">
+      <c r="D24" s="10">
         <v>0.38876150824737099</v>
       </c>
-      <c r="E24" s="92">
+      <c r="E24" s="5">
         <v>9.7642935537949102E-2</v>
       </c>
-      <c r="F24" s="90">
+      <c r="F24" s="4">
         <v>3.9814606771657099</v>
       </c>
-      <c r="G24" s="110" t="s">
+      <c r="G24" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="94" t="s">
+      <c r="I24" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="J24" s="87">
+      <c r="J24" s="14">
         <v>9.8207379389655694E-2</v>
       </c>
-      <c r="K24" s="87">
+      <c r="K24" s="14">
         <v>0.24063340614060799</v>
       </c>
-      <c r="L24" s="89">
+      <c r="L24" s="15">
         <v>-4.8336095435263501E-2</v>
       </c>
-      <c r="M24" s="89">
+      <c r="M24" s="15">
         <v>4.2859419212394598E-2</v>
       </c>
-      <c r="N24" s="87">
+      <c r="N24" s="14">
         <v>-1.1277823247144001</v>
       </c>
-      <c r="O24" s="89">
+      <c r="O24" s="15">
         <v>0.259411859844703</v>
       </c>
-      <c r="Q24" s="94" t="s">
+      <c r="Q24" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="R24" s="87">
+      <c r="R24" s="14">
         <v>0.186781920528337</v>
       </c>
-      <c r="S24" s="87">
+      <c r="S24" s="14">
         <v>0.62083653287280305</v>
       </c>
-      <c r="T24" s="88">
+      <c r="T24" s="22">
         <v>7.0319710480356207E-2</v>
       </c>
-      <c r="U24" s="89">
+      <c r="U24" s="15">
         <v>3.0208318809517101E-2</v>
       </c>
-      <c r="V24" s="87">
+      <c r="V24" s="14">
         <v>2.3278260178518102</v>
       </c>
-      <c r="W24" s="88">
+      <c r="W24" s="22">
         <v>1.99213439444519E-2</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="97" t="s">
+      <c r="A25" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="90">
+      <c r="B25" s="4">
         <v>0.57651066723842403</v>
       </c>
-      <c r="C25" s="90">
+      <c r="C25" s="4">
         <v>0.57651066723842403</v>
       </c>
-      <c r="D25" s="91">
+      <c r="D25" s="10">
         <v>0.34321871899749701</v>
       </c>
-      <c r="E25" s="92">
+      <c r="E25" s="5">
         <v>8.8693580498578894E-2</v>
       </c>
-      <c r="F25" s="90">
+      <c r="F25" s="4">
         <v>3.8697131975971599</v>
       </c>
-      <c r="G25" s="110" t="s">
+      <c r="G25" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="94" t="s">
+      <c r="I25" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="J25" s="87">
+      <c r="J25" s="14">
         <v>8.7920706129776094E-2</v>
       </c>
-      <c r="K25" s="87">
+      <c r="K25" s="14">
         <v>0.58608089905612204</v>
       </c>
-      <c r="L25" s="89">
+      <c r="L25" s="15">
         <v>-5.84422134248474E-2</v>
       </c>
-      <c r="M25" s="89">
+      <c r="M25" s="15">
         <v>3.8233359786043898E-2</v>
       </c>
-      <c r="N25" s="87">
+      <c r="N25" s="14">
         <v>-1.52856598927987</v>
       </c>
-      <c r="O25" s="89">
+      <c r="O25" s="15">
         <v>0.12637207281625701</v>
       </c>
-      <c r="Q25" s="94" t="s">
+      <c r="Q25" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="R25" s="87">
+      <c r="R25" s="14">
         <v>4.3525849005857598E-2</v>
       </c>
-      <c r="S25" s="87">
+      <c r="S25" s="14">
         <v>4.3525849005857598E-2</v>
       </c>
-      <c r="T25" s="89">
+      <c r="T25" s="15">
         <v>2.66444489024498E-2</v>
       </c>
-      <c r="U25" s="89">
+      <c r="U25" s="15">
         <v>3.7659399670451503E-2</v>
       </c>
-      <c r="V25" s="87">
+      <c r="V25" s="14">
         <v>0.70751124913326102</v>
       </c>
-      <c r="W25" s="89">
+      <c r="W25" s="15">
         <v>0.47924882453168499</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="78" t="s">
         <v>125</v>
       </c>
       <c r="B26" s="7">
@@ -7795,51 +7773,51 @@
       <c r="G26" s="12">
         <v>2.9920329633350601E-3</v>
       </c>
-      <c r="I26" s="94" t="s">
+      <c r="I26" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="J26" s="87">
+      <c r="J26" s="14">
         <v>0.22467498765110999</v>
       </c>
-      <c r="K26" s="87">
+      <c r="K26" s="14">
         <v>0.23449139622892201</v>
       </c>
-      <c r="L26" s="89">
+      <c r="L26" s="15">
         <v>-4.9190359922241703E-2</v>
       </c>
-      <c r="M26" s="89">
+      <c r="M26" s="15">
         <v>3.4318528271432398E-2</v>
       </c>
-      <c r="N26" s="87">
+      <c r="N26" s="14">
         <v>-1.43334701107183</v>
       </c>
-      <c r="O26" s="89">
+      <c r="O26" s="15">
         <v>0.15175869343675799</v>
       </c>
-      <c r="Q26" s="94" t="s">
+      <c r="Q26" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="R26" s="87">
+      <c r="R26" s="14">
         <v>2.8851143818738701E-2</v>
       </c>
-      <c r="S26" s="87">
+      <c r="S26" s="14">
         <v>0.36435621422789999</v>
       </c>
-      <c r="T26" s="89">
+      <c r="T26" s="15">
         <v>-2.4883843373679899E-2</v>
       </c>
-      <c r="U26" s="89">
+      <c r="U26" s="15">
         <v>3.5216525149978098E-2</v>
       </c>
-      <c r="V26" s="87">
+      <c r="V26" s="14">
         <v>-0.706595647006795</v>
       </c>
-      <c r="W26" s="89">
+      <c r="W26" s="15">
         <v>0.479817794840393</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I27" s="95" t="s">
+      <c r="I27" s="75" t="s">
         <v>120</v>
       </c>
       <c r="J27" s="18">
@@ -7860,7 +7838,7 @@
       <c r="O27" s="20">
         <v>0.16984067724777799</v>
       </c>
-      <c r="Q27" s="95" t="s">
+      <c r="Q27" s="75" t="s">
         <v>115</v>
       </c>
       <c r="R27" s="18">
@@ -7883,7 +7861,7 @@
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I28" s="96" t="s">
+      <c r="I28" s="76" t="s">
         <v>121</v>
       </c>
       <c r="J28" s="38">
@@ -7901,10 +7879,10 @@
       <c r="N28" s="38">
         <v>5.8678259314861503</v>
       </c>
-      <c r="O28" s="103" t="s">
+      <c r="O28" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="Q28" s="96" t="s">
+      <c r="Q28" s="76" t="s">
         <v>116</v>
       </c>
       <c r="R28" s="38">
@@ -7927,139 +7905,139 @@
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I29" s="97" t="s">
+      <c r="I29" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="J29" s="90">
+      <c r="J29" s="4">
         <v>0.84657551692770605</v>
       </c>
-      <c r="K29" s="90">
+      <c r="K29" s="4">
         <v>0.85346049216935804</v>
       </c>
-      <c r="L29" s="91">
+      <c r="L29" s="10">
         <v>0.49912631275167701</v>
       </c>
-      <c r="M29" s="92">
+      <c r="M29" s="5">
         <v>6.5859265979663198E-2</v>
       </c>
-      <c r="N29" s="90">
+      <c r="N29" s="4">
         <v>7.5786801648503497</v>
       </c>
-      <c r="O29" s="104" t="s">
+      <c r="O29" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="97" t="s">
+      <c r="Q29" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="R29" s="90">
+      <c r="R29" s="4">
         <v>8.5901561933159705E-4</v>
       </c>
-      <c r="S29" s="90">
+      <c r="S29" s="4">
         <v>6.95694665450486E-2</v>
       </c>
-      <c r="T29" s="92">
+      <c r="T29" s="5">
         <v>4.5633440472272104E-3</v>
       </c>
-      <c r="U29" s="92">
+      <c r="U29" s="5">
         <v>4.5282283268598698E-2</v>
       </c>
-      <c r="V29" s="90">
+      <c r="V29" s="4">
         <v>0.100775484755463</v>
       </c>
-      <c r="W29" s="92">
+      <c r="W29" s="5">
         <v>0.91972868808040498</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I30" s="97" t="s">
+      <c r="I30" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="J30" s="90">
+      <c r="J30" s="4">
         <v>0.83453020830011904</v>
       </c>
-      <c r="K30" s="90">
+      <c r="K30" s="4">
         <v>0.84405379021622995</v>
       </c>
-      <c r="L30" s="91">
+      <c r="L30" s="10">
         <v>0.48637159527366203</v>
       </c>
-      <c r="M30" s="92">
+      <c r="M30" s="5">
         <v>6.3392552948514605E-2</v>
       </c>
-      <c r="N30" s="90">
+      <c r="N30" s="4">
         <v>7.6723774741912898</v>
       </c>
-      <c r="O30" s="104" t="s">
+      <c r="O30" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="Q30" s="97" t="s">
+      <c r="Q30" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="R30" s="90">
+      <c r="R30" s="4">
         <v>0.13708332140079299</v>
       </c>
-      <c r="S30" s="90">
+      <c r="S30" s="4">
         <v>0.13708332140079299</v>
       </c>
-      <c r="T30" s="92">
+      <c r="T30" s="5">
         <v>5.3209105457176498E-2</v>
       </c>
-      <c r="U30" s="92">
+      <c r="U30" s="5">
         <v>4.0251469248442397E-2</v>
       </c>
-      <c r="V30" s="90">
+      <c r="V30" s="4">
         <v>1.3219170989450399</v>
       </c>
-      <c r="W30" s="92">
+      <c r="W30" s="5">
         <v>0.18619575791306101</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I31" s="97" t="s">
+      <c r="I31" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="J31" s="90">
+      <c r="J31" s="4">
         <v>0.187971496885177</v>
       </c>
-      <c r="K31" s="90">
+      <c r="K31" s="4">
         <v>0.187971496885177</v>
       </c>
-      <c r="L31" s="92">
+      <c r="L31" s="5">
         <v>0.14431180399246399</v>
       </c>
-      <c r="M31" s="92">
+      <c r="M31" s="5">
         <v>0.11336851883823899</v>
       </c>
-      <c r="N31" s="90">
+      <c r="N31" s="4">
         <v>1.2729442482915101</v>
       </c>
-      <c r="O31" s="92">
+      <c r="O31" s="5">
         <v>0.20303782613763799</v>
       </c>
-      <c r="Q31" s="97" t="s">
+      <c r="Q31" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="R31" s="90">
+      <c r="R31" s="4">
         <v>4.1082040598559001E-2</v>
       </c>
-      <c r="S31" s="90">
+      <c r="S31" s="4">
         <v>0.31416602684086697</v>
       </c>
-      <c r="T31" s="92">
+      <c r="T31" s="5">
         <v>3.0220272736632699E-2</v>
       </c>
-      <c r="U31" s="92">
+      <c r="U31" s="5">
         <v>3.7229356565358002E-2</v>
       </c>
-      <c r="V31" s="90">
+      <c r="V31" s="4">
         <v>0.81173234040667597</v>
       </c>
-      <c r="W31" s="92">
+      <c r="W31" s="5">
         <v>0.416945232950235</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I32" s="98" t="s">
+      <c r="I32" s="78" t="s">
         <v>125</v>
       </c>
       <c r="J32" s="7">
@@ -8077,10 +8055,10 @@
       <c r="N32" s="7">
         <v>3.9923043564154002</v>
       </c>
-      <c r="O32" s="105" t="s">
+      <c r="O32" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Q32" s="98" t="s">
+      <c r="Q32" s="78" t="s">
         <v>120</v>
       </c>
       <c r="R32" s="7">

</xml_diff>